<commit_message>
updates to misc workflows
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexandra.veizu\Documents\Reframework_update_UiPath_Services\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c8dbe943334caa90/Documents/UiPath/MyCustomREF/ProjectName_QueueManager/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3F078705-76E7-4249-884A-B762EA8F1802}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -90,10 +90,6 @@
     <t>Framework</t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -122,6 +118,9 @@
   </si>
   <si>
     <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>Sample_Transactions</t>
   </si>
 </sst>
 </file>
@@ -173,15 +172,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -499,16 +506,1075 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="43.59765625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="43" style="4" customWidth="1"/>
+    <col min="3" max="3" width="81.3984375" style="4" customWidth="1"/>
+    <col min="4" max="26" width="8.73046875" style="4" customWidth="1"/>
+    <col min="27" max="16384" width="14.3984375" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="18">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+    </row>
+    <row r="2" spans="1:26">
+      <c r="A2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="28.5">
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" s="4" customFormat="1"/>
+    <row r="18" s="4" customFormat="1"/>
+    <row r="19" s="4" customFormat="1"/>
+    <row r="20" s="4" customFormat="1"/>
+    <row r="21" s="4" customFormat="1"/>
+    <row r="22" s="4" customFormat="1"/>
+    <row r="23" s="4" customFormat="1"/>
+    <row r="24" s="4" customFormat="1"/>
+    <row r="25" s="4" customFormat="1"/>
+    <row r="26" s="4" customFormat="1"/>
+    <row r="27" s="4" customFormat="1"/>
+    <row r="28" s="4" customFormat="1"/>
+    <row r="29" s="4" customFormat="1"/>
+    <row r="30" s="4" customFormat="1"/>
+    <row r="31" s="4" customFormat="1"/>
+    <row r="32" s="4" customFormat="1"/>
+    <row r="33" s="4" customFormat="1"/>
+    <row r="34" s="4" customFormat="1"/>
+    <row r="35" s="4" customFormat="1"/>
+    <row r="36" s="4" customFormat="1"/>
+    <row r="37" s="4" customFormat="1"/>
+    <row r="38" s="4" customFormat="1"/>
+    <row r="39" s="4" customFormat="1"/>
+    <row r="40" s="4" customFormat="1"/>
+    <row r="41" s="4" customFormat="1"/>
+    <row r="42" s="4" customFormat="1"/>
+    <row r="43" s="4" customFormat="1"/>
+    <row r="44" s="4" customFormat="1"/>
+    <row r="45" s="4" customFormat="1"/>
+    <row r="46" s="4" customFormat="1"/>
+    <row r="47" s="4" customFormat="1"/>
+    <row r="48" s="4" customFormat="1"/>
+    <row r="49" s="4" customFormat="1"/>
+    <row r="50" s="4" customFormat="1"/>
+    <row r="51" s="4" customFormat="1"/>
+    <row r="52" s="4" customFormat="1"/>
+    <row r="53" s="4" customFormat="1"/>
+    <row r="54" s="4" customFormat="1"/>
+    <row r="55" s="4" customFormat="1"/>
+    <row r="56" s="4" customFormat="1"/>
+    <row r="57" s="4" customFormat="1"/>
+    <row r="58" s="4" customFormat="1"/>
+    <row r="59" s="4" customFormat="1"/>
+    <row r="60" s="4" customFormat="1"/>
+    <row r="61" s="4" customFormat="1"/>
+    <row r="62" s="4" customFormat="1"/>
+    <row r="63" s="4" customFormat="1"/>
+    <row r="64" s="4" customFormat="1"/>
+    <row r="65" s="4" customFormat="1"/>
+    <row r="66" s="4" customFormat="1"/>
+    <row r="67" s="4" customFormat="1"/>
+    <row r="68" s="4" customFormat="1"/>
+    <row r="69" s="4" customFormat="1"/>
+    <row r="70" s="4" customFormat="1"/>
+    <row r="71" s="4" customFormat="1"/>
+    <row r="72" s="4" customFormat="1"/>
+    <row r="73" s="4" customFormat="1"/>
+    <row r="74" s="4" customFormat="1"/>
+    <row r="75" s="4" customFormat="1"/>
+    <row r="76" s="4" customFormat="1"/>
+    <row r="77" s="4" customFormat="1"/>
+    <row r="78" s="4" customFormat="1"/>
+    <row r="79" s="4" customFormat="1"/>
+    <row r="80" s="4" customFormat="1"/>
+    <row r="81" s="4" customFormat="1"/>
+    <row r="82" s="4" customFormat="1"/>
+    <row r="83" s="4" customFormat="1"/>
+    <row r="84" s="4" customFormat="1"/>
+    <row r="85" s="4" customFormat="1"/>
+    <row r="86" s="4" customFormat="1"/>
+    <row r="87" s="4" customFormat="1"/>
+    <row r="88" s="4" customFormat="1"/>
+    <row r="89" s="4" customFormat="1"/>
+    <row r="90" s="4" customFormat="1"/>
+    <row r="91" s="4" customFormat="1"/>
+    <row r="92" s="4" customFormat="1"/>
+    <row r="93" s="4" customFormat="1"/>
+    <row r="94" s="4" customFormat="1"/>
+    <row r="95" s="4" customFormat="1"/>
+    <row r="96" s="4" customFormat="1"/>
+    <row r="97" s="4" customFormat="1"/>
+    <row r="98" s="4" customFormat="1"/>
+    <row r="99" s="4" customFormat="1"/>
+    <row r="100" s="4" customFormat="1"/>
+    <row r="101" s="4" customFormat="1"/>
+    <row r="102" s="4" customFormat="1"/>
+    <row r="103" s="4" customFormat="1"/>
+    <row r="104" s="4" customFormat="1"/>
+    <row r="105" s="4" customFormat="1"/>
+    <row r="106" s="4" customFormat="1"/>
+    <row r="107" s="4" customFormat="1"/>
+    <row r="108" s="4" customFormat="1"/>
+    <row r="109" s="4" customFormat="1"/>
+    <row r="110" s="4" customFormat="1"/>
+    <row r="111" s="4" customFormat="1"/>
+    <row r="112" s="4" customFormat="1"/>
+    <row r="113" s="4" customFormat="1"/>
+    <row r="114" s="4" customFormat="1"/>
+    <row r="115" s="4" customFormat="1"/>
+    <row r="116" s="4" customFormat="1"/>
+    <row r="117" s="4" customFormat="1"/>
+    <row r="118" s="4" customFormat="1"/>
+    <row r="119" s="4" customFormat="1"/>
+    <row r="120" s="4" customFormat="1"/>
+    <row r="121" s="4" customFormat="1"/>
+    <row r="122" s="4" customFormat="1"/>
+    <row r="123" s="4" customFormat="1"/>
+    <row r="124" s="4" customFormat="1"/>
+    <row r="125" s="4" customFormat="1"/>
+    <row r="126" s="4" customFormat="1"/>
+    <row r="127" s="4" customFormat="1"/>
+    <row r="128" s="4" customFormat="1"/>
+    <row r="129" s="4" customFormat="1"/>
+    <row r="130" s="4" customFormat="1"/>
+    <row r="131" s="4" customFormat="1"/>
+    <row r="132" s="4" customFormat="1"/>
+    <row r="133" s="4" customFormat="1"/>
+    <row r="134" s="4" customFormat="1"/>
+    <row r="135" s="4" customFormat="1"/>
+    <row r="136" s="4" customFormat="1"/>
+    <row r="137" s="4" customFormat="1"/>
+    <row r="138" s="4" customFormat="1"/>
+    <row r="139" s="4" customFormat="1"/>
+    <row r="140" s="4" customFormat="1"/>
+    <row r="141" s="4" customFormat="1"/>
+    <row r="142" s="4" customFormat="1"/>
+    <row r="143" s="4" customFormat="1"/>
+    <row r="144" s="4" customFormat="1"/>
+    <row r="145" s="4" customFormat="1"/>
+    <row r="146" s="4" customFormat="1"/>
+    <row r="147" s="4" customFormat="1"/>
+    <row r="148" s="4" customFormat="1"/>
+    <row r="149" s="4" customFormat="1"/>
+    <row r="150" s="4" customFormat="1"/>
+    <row r="151" s="4" customFormat="1"/>
+    <row r="152" s="4" customFormat="1"/>
+    <row r="153" s="4" customFormat="1"/>
+    <row r="154" s="4" customFormat="1"/>
+    <row r="155" s="4" customFormat="1"/>
+    <row r="156" s="4" customFormat="1"/>
+    <row r="157" s="4" customFormat="1"/>
+    <row r="158" s="4" customFormat="1"/>
+    <row r="159" s="4" customFormat="1"/>
+    <row r="160" s="4" customFormat="1"/>
+    <row r="161" s="4" customFormat="1"/>
+    <row r="162" s="4" customFormat="1"/>
+    <row r="163" s="4" customFormat="1"/>
+    <row r="164" s="4" customFormat="1"/>
+    <row r="165" s="4" customFormat="1"/>
+    <row r="166" s="4" customFormat="1"/>
+    <row r="167" s="4" customFormat="1"/>
+    <row r="168" s="4" customFormat="1"/>
+    <row r="169" s="4" customFormat="1"/>
+    <row r="170" s="4" customFormat="1"/>
+    <row r="171" s="4" customFormat="1"/>
+    <row r="172" s="4" customFormat="1"/>
+    <row r="173" s="4" customFormat="1"/>
+    <row r="174" s="4" customFormat="1"/>
+    <row r="175" s="4" customFormat="1"/>
+    <row r="176" s="4" customFormat="1"/>
+    <row r="177" s="4" customFormat="1"/>
+    <row r="178" s="4" customFormat="1"/>
+    <row r="179" s="4" customFormat="1"/>
+    <row r="180" s="4" customFormat="1"/>
+    <row r="181" s="4" customFormat="1"/>
+    <row r="182" s="4" customFormat="1"/>
+    <row r="183" s="4" customFormat="1"/>
+    <row r="184" s="4" customFormat="1"/>
+    <row r="185" s="4" customFormat="1"/>
+    <row r="186" s="4" customFormat="1"/>
+    <row r="187" s="4" customFormat="1"/>
+    <row r="188" s="4" customFormat="1"/>
+    <row r="189" s="4" customFormat="1"/>
+    <row r="190" s="4" customFormat="1"/>
+    <row r="191" s="4" customFormat="1"/>
+    <row r="192" s="4" customFormat="1"/>
+    <row r="193" s="4" customFormat="1"/>
+    <row r="194" s="4" customFormat="1"/>
+    <row r="195" s="4" customFormat="1"/>
+    <row r="196" s="4" customFormat="1"/>
+    <row r="197" s="4" customFormat="1"/>
+    <row r="198" s="4" customFormat="1"/>
+    <row r="199" s="4" customFormat="1"/>
+    <row r="200" s="4" customFormat="1"/>
+    <row r="201" s="4" customFormat="1"/>
+    <row r="202" s="4" customFormat="1"/>
+    <row r="203" s="4" customFormat="1"/>
+    <row r="204" s="4" customFormat="1"/>
+    <row r="205" s="4" customFormat="1"/>
+    <row r="206" s="4" customFormat="1"/>
+    <row r="207" s="4" customFormat="1"/>
+    <row r="208" s="4" customFormat="1"/>
+    <row r="209" s="4" customFormat="1"/>
+    <row r="210" s="4" customFormat="1"/>
+    <row r="211" s="4" customFormat="1"/>
+    <row r="212" s="4" customFormat="1"/>
+    <row r="213" s="4" customFormat="1"/>
+    <row r="214" s="4" customFormat="1"/>
+    <row r="215" s="4" customFormat="1"/>
+    <row r="216" s="4" customFormat="1"/>
+    <row r="217" s="4" customFormat="1"/>
+    <row r="218" s="4" customFormat="1"/>
+    <row r="219" s="4" customFormat="1"/>
+    <row r="220" s="4" customFormat="1"/>
+    <row r="221" s="4" customFormat="1"/>
+    <row r="222" s="4" customFormat="1"/>
+    <row r="223" s="4" customFormat="1"/>
+    <row r="224" s="4" customFormat="1"/>
+    <row r="225" s="4" customFormat="1"/>
+    <row r="226" s="4" customFormat="1"/>
+    <row r="227" s="4" customFormat="1"/>
+    <row r="228" s="4" customFormat="1"/>
+    <row r="229" s="4" customFormat="1"/>
+    <row r="230" s="4" customFormat="1"/>
+    <row r="231" s="4" customFormat="1"/>
+    <row r="232" s="4" customFormat="1"/>
+    <row r="233" s="4" customFormat="1"/>
+    <row r="234" s="4" customFormat="1"/>
+    <row r="235" s="4" customFormat="1"/>
+    <row r="236" s="4" customFormat="1"/>
+    <row r="237" s="4" customFormat="1"/>
+    <row r="238" s="4" customFormat="1"/>
+    <row r="239" s="4" customFormat="1"/>
+    <row r="240" s="4" customFormat="1"/>
+    <row r="241" s="4" customFormat="1"/>
+    <row r="242" s="4" customFormat="1"/>
+    <row r="243" s="4" customFormat="1"/>
+    <row r="244" s="4" customFormat="1"/>
+    <row r="245" s="4" customFormat="1"/>
+    <row r="246" s="4" customFormat="1"/>
+    <row r="247" s="4" customFormat="1"/>
+    <row r="248" s="4" customFormat="1"/>
+    <row r="249" s="4" customFormat="1"/>
+    <row r="250" s="4" customFormat="1"/>
+    <row r="251" s="4" customFormat="1"/>
+    <row r="252" s="4" customFormat="1"/>
+    <row r="253" s="4" customFormat="1"/>
+    <row r="254" s="4" customFormat="1"/>
+    <row r="255" s="4" customFormat="1"/>
+    <row r="256" s="4" customFormat="1"/>
+    <row r="257" s="4" customFormat="1"/>
+    <row r="258" s="4" customFormat="1"/>
+    <row r="259" s="4" customFormat="1"/>
+    <row r="260" s="4" customFormat="1"/>
+    <row r="261" s="4" customFormat="1"/>
+    <row r="262" s="4" customFormat="1"/>
+    <row r="263" s="4" customFormat="1"/>
+    <row r="264" s="4" customFormat="1"/>
+    <row r="265" s="4" customFormat="1"/>
+    <row r="266" s="4" customFormat="1"/>
+    <row r="267" s="4" customFormat="1"/>
+    <row r="268" s="4" customFormat="1"/>
+    <row r="269" s="4" customFormat="1"/>
+    <row r="270" s="4" customFormat="1"/>
+    <row r="271" s="4" customFormat="1"/>
+    <row r="272" s="4" customFormat="1"/>
+    <row r="273" s="4" customFormat="1"/>
+    <row r="274" s="4" customFormat="1"/>
+    <row r="275" s="4" customFormat="1"/>
+    <row r="276" s="4" customFormat="1"/>
+    <row r="277" s="4" customFormat="1"/>
+    <row r="278" s="4" customFormat="1"/>
+    <row r="279" s="4" customFormat="1"/>
+    <row r="280" s="4" customFormat="1"/>
+    <row r="281" s="4" customFormat="1"/>
+    <row r="282" s="4" customFormat="1"/>
+    <row r="283" s="4" customFormat="1"/>
+    <row r="284" s="4" customFormat="1"/>
+    <row r="285" s="4" customFormat="1"/>
+    <row r="286" s="4" customFormat="1"/>
+    <row r="287" s="4" customFormat="1"/>
+    <row r="288" s="4" customFormat="1"/>
+    <row r="289" s="4" customFormat="1"/>
+    <row r="290" s="4" customFormat="1"/>
+    <row r="291" s="4" customFormat="1"/>
+    <row r="292" s="4" customFormat="1"/>
+    <row r="293" s="4" customFormat="1"/>
+    <row r="294" s="4" customFormat="1"/>
+    <row r="295" s="4" customFormat="1"/>
+    <row r="296" s="4" customFormat="1"/>
+    <row r="297" s="4" customFormat="1"/>
+    <row r="298" s="4" customFormat="1"/>
+    <row r="299" s="4" customFormat="1"/>
+    <row r="300" s="4" customFormat="1"/>
+    <row r="301" s="4" customFormat="1"/>
+    <row r="302" s="4" customFormat="1"/>
+    <row r="303" s="4" customFormat="1"/>
+    <row r="304" s="4" customFormat="1"/>
+    <row r="305" s="4" customFormat="1"/>
+    <row r="306" s="4" customFormat="1"/>
+    <row r="307" s="4" customFormat="1"/>
+    <row r="308" s="4" customFormat="1"/>
+    <row r="309" s="4" customFormat="1"/>
+    <row r="310" s="4" customFormat="1"/>
+    <row r="311" s="4" customFormat="1"/>
+    <row r="312" s="4" customFormat="1"/>
+    <row r="313" s="4" customFormat="1"/>
+    <row r="314" s="4" customFormat="1"/>
+    <row r="315" s="4" customFormat="1"/>
+    <row r="316" s="4" customFormat="1"/>
+    <row r="317" s="4" customFormat="1"/>
+    <row r="318" s="4" customFormat="1"/>
+    <row r="319" s="4" customFormat="1"/>
+    <row r="320" s="4" customFormat="1"/>
+    <row r="321" s="4" customFormat="1"/>
+    <row r="322" s="4" customFormat="1"/>
+    <row r="323" s="4" customFormat="1"/>
+    <row r="324" s="4" customFormat="1"/>
+    <row r="325" s="4" customFormat="1"/>
+    <row r="326" s="4" customFormat="1"/>
+    <row r="327" s="4" customFormat="1"/>
+    <row r="328" s="4" customFormat="1"/>
+    <row r="329" s="4" customFormat="1"/>
+    <row r="330" s="4" customFormat="1"/>
+    <row r="331" s="4" customFormat="1"/>
+    <row r="332" s="4" customFormat="1"/>
+    <row r="333" s="4" customFormat="1"/>
+    <row r="334" s="4" customFormat="1"/>
+    <row r="335" s="4" customFormat="1"/>
+    <row r="336" s="4" customFormat="1"/>
+    <row r="337" s="4" customFormat="1"/>
+    <row r="338" s="4" customFormat="1"/>
+    <row r="339" s="4" customFormat="1"/>
+    <row r="340" s="4" customFormat="1"/>
+    <row r="341" s="4" customFormat="1"/>
+    <row r="342" s="4" customFormat="1"/>
+    <row r="343" s="4" customFormat="1"/>
+    <row r="344" s="4" customFormat="1"/>
+    <row r="345" s="4" customFormat="1"/>
+    <row r="346" s="4" customFormat="1"/>
+    <row r="347" s="4" customFormat="1"/>
+    <row r="348" s="4" customFormat="1"/>
+    <row r="349" s="4" customFormat="1"/>
+    <row r="350" s="4" customFormat="1"/>
+    <row r="351" s="4" customFormat="1"/>
+    <row r="352" s="4" customFormat="1"/>
+    <row r="353" s="4" customFormat="1"/>
+    <row r="354" s="4" customFormat="1"/>
+    <row r="355" s="4" customFormat="1"/>
+    <row r="356" s="4" customFormat="1"/>
+    <row r="357" s="4" customFormat="1"/>
+    <row r="358" s="4" customFormat="1"/>
+    <row r="359" s="4" customFormat="1"/>
+    <row r="360" s="4" customFormat="1"/>
+    <row r="361" s="4" customFormat="1"/>
+    <row r="362" s="4" customFormat="1"/>
+    <row r="363" s="4" customFormat="1"/>
+    <row r="364" s="4" customFormat="1"/>
+    <row r="365" s="4" customFormat="1"/>
+    <row r="366" s="4" customFormat="1"/>
+    <row r="367" s="4" customFormat="1"/>
+    <row r="368" s="4" customFormat="1"/>
+    <row r="369" s="4" customFormat="1"/>
+    <row r="370" s="4" customFormat="1"/>
+    <row r="371" s="4" customFormat="1"/>
+    <row r="372" s="4" customFormat="1"/>
+    <row r="373" s="4" customFormat="1"/>
+    <row r="374" s="4" customFormat="1"/>
+    <row r="375" s="4" customFormat="1"/>
+    <row r="376" s="4" customFormat="1"/>
+    <row r="377" s="4" customFormat="1"/>
+    <row r="378" s="4" customFormat="1"/>
+    <row r="379" s="4" customFormat="1"/>
+    <row r="380" s="4" customFormat="1"/>
+    <row r="381" s="4" customFormat="1"/>
+    <row r="382" s="4" customFormat="1"/>
+    <row r="383" s="4" customFormat="1"/>
+    <row r="384" s="4" customFormat="1"/>
+    <row r="385" s="4" customFormat="1"/>
+    <row r="386" s="4" customFormat="1"/>
+    <row r="387" s="4" customFormat="1"/>
+    <row r="388" s="4" customFormat="1"/>
+    <row r="389" s="4" customFormat="1"/>
+    <row r="390" s="4" customFormat="1"/>
+    <row r="391" s="4" customFormat="1"/>
+    <row r="392" s="4" customFormat="1"/>
+    <row r="393" s="4" customFormat="1"/>
+    <row r="394" s="4" customFormat="1"/>
+    <row r="395" s="4" customFormat="1"/>
+    <row r="396" s="4" customFormat="1"/>
+    <row r="397" s="4" customFormat="1"/>
+    <row r="398" s="4" customFormat="1"/>
+    <row r="399" s="4" customFormat="1"/>
+    <row r="400" s="4" customFormat="1"/>
+    <row r="401" s="4" customFormat="1"/>
+    <row r="402" s="4" customFormat="1"/>
+    <row r="403" s="4" customFormat="1"/>
+    <row r="404" s="4" customFormat="1"/>
+    <row r="405" s="4" customFormat="1"/>
+    <row r="406" s="4" customFormat="1"/>
+    <row r="407" s="4" customFormat="1"/>
+    <row r="408" s="4" customFormat="1"/>
+    <row r="409" s="4" customFormat="1"/>
+    <row r="410" s="4" customFormat="1"/>
+    <row r="411" s="4" customFormat="1"/>
+    <row r="412" s="4" customFormat="1"/>
+    <row r="413" s="4" customFormat="1"/>
+    <row r="414" s="4" customFormat="1"/>
+    <row r="415" s="4" customFormat="1"/>
+    <row r="416" s="4" customFormat="1"/>
+    <row r="417" s="4" customFormat="1"/>
+    <row r="418" s="4" customFormat="1"/>
+    <row r="419" s="4" customFormat="1"/>
+    <row r="420" s="4" customFormat="1"/>
+    <row r="421" s="4" customFormat="1"/>
+    <row r="422" s="4" customFormat="1"/>
+    <row r="423" s="4" customFormat="1"/>
+    <row r="424" s="4" customFormat="1"/>
+    <row r="425" s="4" customFormat="1"/>
+    <row r="426" s="4" customFormat="1"/>
+    <row r="427" s="4" customFormat="1"/>
+    <row r="428" s="4" customFormat="1"/>
+    <row r="429" s="4" customFormat="1"/>
+    <row r="430" s="4" customFormat="1"/>
+    <row r="431" s="4" customFormat="1"/>
+    <row r="432" s="4" customFormat="1"/>
+    <row r="433" s="4" customFormat="1"/>
+    <row r="434" s="4" customFormat="1"/>
+    <row r="435" s="4" customFormat="1"/>
+    <row r="436" s="4" customFormat="1"/>
+    <row r="437" s="4" customFormat="1"/>
+    <row r="438" s="4" customFormat="1"/>
+    <row r="439" s="4" customFormat="1"/>
+    <row r="440" s="4" customFormat="1"/>
+    <row r="441" s="4" customFormat="1"/>
+    <row r="442" s="4" customFormat="1"/>
+    <row r="443" s="4" customFormat="1"/>
+    <row r="444" s="4" customFormat="1"/>
+    <row r="445" s="4" customFormat="1"/>
+    <row r="446" s="4" customFormat="1"/>
+    <row r="447" s="4" customFormat="1"/>
+    <row r="448" s="4" customFormat="1"/>
+    <row r="449" s="4" customFormat="1"/>
+    <row r="450" s="4" customFormat="1"/>
+    <row r="451" s="4" customFormat="1"/>
+    <row r="452" s="4" customFormat="1"/>
+    <row r="453" s="4" customFormat="1"/>
+    <row r="454" s="4" customFormat="1"/>
+    <row r="455" s="4" customFormat="1"/>
+    <row r="456" s="4" customFormat="1"/>
+    <row r="457" s="4" customFormat="1"/>
+    <row r="458" s="4" customFormat="1"/>
+    <row r="459" s="4" customFormat="1"/>
+    <row r="460" s="4" customFormat="1"/>
+    <row r="461" s="4" customFormat="1"/>
+    <row r="462" s="4" customFormat="1"/>
+    <row r="463" s="4" customFormat="1"/>
+    <row r="464" s="4" customFormat="1"/>
+    <row r="465" s="4" customFormat="1"/>
+    <row r="466" s="4" customFormat="1"/>
+    <row r="467" s="4" customFormat="1"/>
+    <row r="468" s="4" customFormat="1"/>
+    <row r="469" s="4" customFormat="1"/>
+    <row r="470" s="4" customFormat="1"/>
+    <row r="471" s="4" customFormat="1"/>
+    <row r="472" s="4" customFormat="1"/>
+    <row r="473" s="4" customFormat="1"/>
+    <row r="474" s="4" customFormat="1"/>
+    <row r="475" s="4" customFormat="1"/>
+    <row r="476" s="4" customFormat="1"/>
+    <row r="477" s="4" customFormat="1"/>
+    <row r="478" s="4" customFormat="1"/>
+    <row r="479" s="4" customFormat="1"/>
+    <row r="480" s="4" customFormat="1"/>
+    <row r="481" s="4" customFormat="1"/>
+    <row r="482" s="4" customFormat="1"/>
+    <row r="483" s="4" customFormat="1"/>
+    <row r="484" s="4" customFormat="1"/>
+    <row r="485" s="4" customFormat="1"/>
+    <row r="486" s="4" customFormat="1"/>
+    <row r="487" s="4" customFormat="1"/>
+    <row r="488" s="4" customFormat="1"/>
+    <row r="489" s="4" customFormat="1"/>
+    <row r="490" s="4" customFormat="1"/>
+    <row r="491" s="4" customFormat="1"/>
+    <row r="492" s="4" customFormat="1"/>
+    <row r="493" s="4" customFormat="1"/>
+    <row r="494" s="4" customFormat="1"/>
+    <row r="495" s="4" customFormat="1"/>
+    <row r="496" s="4" customFormat="1"/>
+    <row r="497" s="4" customFormat="1"/>
+    <row r="498" s="4" customFormat="1"/>
+    <row r="499" s="4" customFormat="1"/>
+    <row r="500" s="4" customFormat="1"/>
+    <row r="501" s="4" customFormat="1"/>
+    <row r="502" s="4" customFormat="1"/>
+    <row r="503" s="4" customFormat="1"/>
+    <row r="504" s="4" customFormat="1"/>
+    <row r="505" s="4" customFormat="1"/>
+    <row r="506" s="4" customFormat="1"/>
+    <row r="507" s="4" customFormat="1"/>
+    <row r="508" s="4" customFormat="1"/>
+    <row r="509" s="4" customFormat="1"/>
+    <row r="510" s="4" customFormat="1"/>
+    <row r="511" s="4" customFormat="1"/>
+    <row r="512" s="4" customFormat="1"/>
+    <row r="513" s="4" customFormat="1"/>
+    <row r="514" s="4" customFormat="1"/>
+    <row r="515" s="4" customFormat="1"/>
+    <row r="516" s="4" customFormat="1"/>
+    <row r="517" s="4" customFormat="1"/>
+    <row r="518" s="4" customFormat="1"/>
+    <row r="519" s="4" customFormat="1"/>
+    <row r="520" s="4" customFormat="1"/>
+    <row r="521" s="4" customFormat="1"/>
+    <row r="522" s="4" customFormat="1"/>
+    <row r="523" s="4" customFormat="1"/>
+    <row r="524" s="4" customFormat="1"/>
+    <row r="525" s="4" customFormat="1"/>
+    <row r="526" s="4" customFormat="1"/>
+    <row r="527" s="4" customFormat="1"/>
+    <row r="528" s="4" customFormat="1"/>
+    <row r="529" s="4" customFormat="1"/>
+    <row r="530" s="4" customFormat="1"/>
+    <row r="531" s="4" customFormat="1"/>
+    <row r="532" s="4" customFormat="1"/>
+    <row r="533" s="4" customFormat="1"/>
+    <row r="534" s="4" customFormat="1"/>
+    <row r="535" s="4" customFormat="1"/>
+    <row r="536" s="4" customFormat="1"/>
+    <row r="537" s="4" customFormat="1"/>
+    <row r="538" s="4" customFormat="1"/>
+    <row r="539" s="4" customFormat="1"/>
+    <row r="540" s="4" customFormat="1"/>
+    <row r="541" s="4" customFormat="1"/>
+    <row r="542" s="4" customFormat="1"/>
+    <row r="543" s="4" customFormat="1"/>
+    <row r="544" s="4" customFormat="1"/>
+    <row r="545" s="4" customFormat="1"/>
+    <row r="546" s="4" customFormat="1"/>
+    <row r="547" s="4" customFormat="1"/>
+    <row r="548" s="4" customFormat="1"/>
+    <row r="549" s="4" customFormat="1"/>
+    <row r="550" s="4" customFormat="1"/>
+    <row r="551" s="4" customFormat="1"/>
+    <row r="552" s="4" customFormat="1"/>
+    <row r="553" s="4" customFormat="1"/>
+    <row r="554" s="4" customFormat="1"/>
+    <row r="555" s="4" customFormat="1"/>
+    <row r="556" s="4" customFormat="1"/>
+    <row r="557" s="4" customFormat="1"/>
+    <row r="558" s="4" customFormat="1"/>
+    <row r="559" s="4" customFormat="1"/>
+    <row r="560" s="4" customFormat="1"/>
+    <row r="561" s="4" customFormat="1"/>
+    <row r="562" s="4" customFormat="1"/>
+    <row r="563" s="4" customFormat="1"/>
+    <row r="564" s="4" customFormat="1"/>
+    <row r="565" s="4" customFormat="1"/>
+    <row r="566" s="4" customFormat="1"/>
+    <row r="567" s="4" customFormat="1"/>
+    <row r="568" s="4" customFormat="1"/>
+    <row r="569" s="4" customFormat="1"/>
+    <row r="570" s="4" customFormat="1"/>
+    <row r="571" s="4" customFormat="1"/>
+    <row r="572" s="4" customFormat="1"/>
+    <row r="573" s="4" customFormat="1"/>
+    <row r="574" s="4" customFormat="1"/>
+    <row r="575" s="4" customFormat="1"/>
+    <row r="576" s="4" customFormat="1"/>
+    <row r="577" s="4" customFormat="1"/>
+    <row r="578" s="4" customFormat="1"/>
+    <row r="579" s="4" customFormat="1"/>
+    <row r="580" s="4" customFormat="1"/>
+    <row r="581" s="4" customFormat="1"/>
+    <row r="582" s="4" customFormat="1"/>
+    <row r="583" s="4" customFormat="1"/>
+    <row r="584" s="4" customFormat="1"/>
+    <row r="585" s="4" customFormat="1"/>
+    <row r="586" s="4" customFormat="1"/>
+    <row r="587" s="4" customFormat="1"/>
+    <row r="588" s="4" customFormat="1"/>
+    <row r="589" s="4" customFormat="1"/>
+    <row r="590" s="4" customFormat="1"/>
+    <row r="591" s="4" customFormat="1"/>
+    <row r="592" s="4" customFormat="1"/>
+    <row r="593" s="4" customFormat="1"/>
+    <row r="594" s="4" customFormat="1"/>
+    <row r="595" s="4" customFormat="1"/>
+    <row r="596" s="4" customFormat="1"/>
+    <row r="597" s="4" customFormat="1"/>
+    <row r="598" s="4" customFormat="1"/>
+    <row r="599" s="4" customFormat="1"/>
+    <row r="600" s="4" customFormat="1"/>
+    <row r="601" s="4" customFormat="1"/>
+    <row r="602" s="4" customFormat="1"/>
+    <row r="603" s="4" customFormat="1"/>
+    <row r="604" s="4" customFormat="1"/>
+    <row r="605" s="4" customFormat="1"/>
+    <row r="606" s="4" customFormat="1"/>
+    <row r="607" s="4" customFormat="1"/>
+    <row r="608" s="4" customFormat="1"/>
+    <row r="609" s="4" customFormat="1"/>
+    <row r="610" s="4" customFormat="1"/>
+    <row r="611" s="4" customFormat="1"/>
+    <row r="612" s="4" customFormat="1"/>
+    <row r="613" s="4" customFormat="1"/>
+    <row r="614" s="4" customFormat="1"/>
+    <row r="615" s="4" customFormat="1"/>
+    <row r="616" s="4" customFormat="1"/>
+    <row r="617" s="4" customFormat="1"/>
+    <row r="618" s="4" customFormat="1"/>
+    <row r="619" s="4" customFormat="1"/>
+    <row r="620" s="4" customFormat="1"/>
+    <row r="621" s="4" customFormat="1"/>
+    <row r="622" s="4" customFormat="1"/>
+    <row r="623" s="4" customFormat="1"/>
+    <row r="624" s="4" customFormat="1"/>
+    <row r="625" s="4" customFormat="1"/>
+    <row r="626" s="4" customFormat="1"/>
+    <row r="627" s="4" customFormat="1"/>
+    <row r="628" s="4" customFormat="1"/>
+    <row r="629" s="4" customFormat="1"/>
+    <row r="630" s="4" customFormat="1"/>
+    <row r="631" s="4" customFormat="1"/>
+    <row r="632" s="4" customFormat="1"/>
+    <row r="633" s="4" customFormat="1"/>
+    <row r="634" s="4" customFormat="1"/>
+    <row r="635" s="4" customFormat="1"/>
+    <row r="636" s="4" customFormat="1"/>
+    <row r="637" s="4" customFormat="1"/>
+    <row r="638" s="4" customFormat="1"/>
+    <row r="639" s="4" customFormat="1"/>
+    <row r="640" s="4" customFormat="1"/>
+    <row r="641" s="4" customFormat="1"/>
+    <row r="642" s="4" customFormat="1"/>
+    <row r="643" s="4" customFormat="1"/>
+    <row r="644" s="4" customFormat="1"/>
+    <row r="645" s="4" customFormat="1"/>
+    <row r="646" s="4" customFormat="1"/>
+    <row r="647" s="4" customFormat="1"/>
+    <row r="648" s="4" customFormat="1"/>
+    <row r="649" s="4" customFormat="1"/>
+    <row r="650" s="4" customFormat="1"/>
+    <row r="651" s="4" customFormat="1"/>
+    <row r="652" s="4" customFormat="1"/>
+    <row r="653" s="4" customFormat="1"/>
+    <row r="654" s="4" customFormat="1"/>
+    <row r="655" s="4" customFormat="1"/>
+    <row r="656" s="4" customFormat="1"/>
+    <row r="657" s="4" customFormat="1"/>
+    <row r="658" s="4" customFormat="1"/>
+    <row r="659" s="4" customFormat="1"/>
+    <row r="660" s="4" customFormat="1"/>
+    <row r="661" s="4" customFormat="1"/>
+    <row r="662" s="4" customFormat="1"/>
+    <row r="663" s="4" customFormat="1"/>
+    <row r="664" s="4" customFormat="1"/>
+    <row r="665" s="4" customFormat="1"/>
+    <row r="666" s="4" customFormat="1"/>
+    <row r="667" s="4" customFormat="1"/>
+    <row r="668" s="4" customFormat="1"/>
+    <row r="669" s="4" customFormat="1"/>
+    <row r="670" s="4" customFormat="1"/>
+    <row r="671" s="4" customFormat="1"/>
+    <row r="672" s="4" customFormat="1"/>
+    <row r="673" s="4" customFormat="1"/>
+    <row r="674" s="4" customFormat="1"/>
+    <row r="675" s="4" customFormat="1"/>
+    <row r="676" s="4" customFormat="1"/>
+    <row r="677" s="4" customFormat="1"/>
+    <row r="678" s="4" customFormat="1"/>
+    <row r="679" s="4" customFormat="1"/>
+    <row r="680" s="4" customFormat="1"/>
+    <row r="681" s="4" customFormat="1"/>
+    <row r="682" s="4" customFormat="1"/>
+    <row r="683" s="4" customFormat="1"/>
+    <row r="684" s="4" customFormat="1"/>
+    <row r="685" s="4" customFormat="1"/>
+    <row r="686" s="4" customFormat="1"/>
+    <row r="687" s="4" customFormat="1"/>
+    <row r="688" s="4" customFormat="1"/>
+    <row r="689" s="4" customFormat="1"/>
+    <row r="690" s="4" customFormat="1"/>
+    <row r="691" s="4" customFormat="1"/>
+    <row r="692" s="4" customFormat="1"/>
+    <row r="693" s="4" customFormat="1"/>
+    <row r="694" s="4" customFormat="1"/>
+    <row r="695" s="4" customFormat="1"/>
+    <row r="696" s="4" customFormat="1"/>
+    <row r="697" s="4" customFormat="1"/>
+    <row r="698" s="4" customFormat="1"/>
+    <row r="699" s="4" customFormat="1"/>
+    <row r="700" s="4" customFormat="1"/>
+    <row r="701" s="4" customFormat="1"/>
+    <row r="702" s="4" customFormat="1"/>
+    <row r="703" s="4" customFormat="1"/>
+    <row r="704" s="4" customFormat="1"/>
+    <row r="705" s="4" customFormat="1"/>
+    <row r="706" s="4" customFormat="1"/>
+    <row r="707" s="4" customFormat="1"/>
+    <row r="708" s="4" customFormat="1"/>
+    <row r="709" s="4" customFormat="1"/>
+    <row r="710" s="4" customFormat="1"/>
+    <row r="711" s="4" customFormat="1"/>
+    <row r="712" s="4" customFormat="1"/>
+    <row r="713" s="4" customFormat="1"/>
+    <row r="714" s="4" customFormat="1"/>
+    <row r="715" s="4" customFormat="1"/>
+    <row r="716" s="4" customFormat="1"/>
+    <row r="717" s="4" customFormat="1"/>
+    <row r="718" s="4" customFormat="1"/>
+    <row r="719" s="4" customFormat="1"/>
+    <row r="720" s="4" customFormat="1"/>
+    <row r="721" s="4" customFormat="1"/>
+    <row r="722" s="4" customFormat="1"/>
+    <row r="723" s="4" customFormat="1"/>
+    <row r="724" s="4" customFormat="1"/>
+    <row r="725" s="4" customFormat="1"/>
+    <row r="726" s="4" customFormat="1"/>
+    <row r="727" s="4" customFormat="1"/>
+    <row r="728" s="4" customFormat="1"/>
+    <row r="729" s="4" customFormat="1"/>
+    <row r="730" s="4" customFormat="1"/>
+    <row r="731" s="4" customFormat="1"/>
+    <row r="732" s="4" customFormat="1"/>
+    <row r="733" s="4" customFormat="1"/>
+    <row r="734" s="4" customFormat="1"/>
+    <row r="735" s="4" customFormat="1"/>
+    <row r="736" s="4" customFormat="1"/>
+    <row r="737" s="4" customFormat="1"/>
+    <row r="738" s="4" customFormat="1"/>
+    <row r="739" s="4" customFormat="1"/>
+    <row r="740" s="4" customFormat="1"/>
+    <row r="741" s="4" customFormat="1"/>
+    <row r="742" s="4" customFormat="1"/>
+    <row r="743" s="4" customFormat="1"/>
+    <row r="744" s="4" customFormat="1"/>
+    <row r="745" s="4" customFormat="1"/>
+    <row r="746" s="4" customFormat="1"/>
+    <row r="747" s="4" customFormat="1"/>
+    <row r="748" s="4" customFormat="1"/>
+    <row r="749" s="4" customFormat="1"/>
+    <row r="750" s="4" customFormat="1"/>
+    <row r="751" s="4" customFormat="1"/>
+    <row r="752" s="4" customFormat="1"/>
+    <row r="753" s="4" customFormat="1"/>
+    <row r="754" s="4" customFormat="1"/>
+    <row r="755" s="4" customFormat="1"/>
+    <row r="756" s="4" customFormat="1"/>
+    <row r="757" s="4" customFormat="1"/>
+    <row r="758" s="4" customFormat="1"/>
+    <row r="759" s="4" customFormat="1"/>
+    <row r="760" s="4" customFormat="1"/>
+    <row r="761" s="4" customFormat="1"/>
+    <row r="762" s="4" customFormat="1"/>
+    <row r="763" s="4" customFormat="1"/>
+    <row r="764" s="4" customFormat="1"/>
+    <row r="765" s="4" customFormat="1"/>
+    <row r="766" s="4" customFormat="1"/>
+    <row r="767" s="4" customFormat="1"/>
+    <row r="768" s="4" customFormat="1"/>
+    <row r="769" s="4" customFormat="1"/>
+    <row r="770" s="4" customFormat="1"/>
+    <row r="771" s="4" customFormat="1"/>
+    <row r="772" s="4" customFormat="1"/>
+    <row r="773" s="4" customFormat="1"/>
+    <row r="774" s="4" customFormat="1"/>
+    <row r="775" s="4" customFormat="1"/>
+    <row r="776" s="4" customFormat="1"/>
+    <row r="777" s="4" customFormat="1"/>
+    <row r="778" s="4" customFormat="1"/>
+    <row r="779" s="4" customFormat="1"/>
+    <row r="780" s="4" customFormat="1"/>
+    <row r="781" s="4" customFormat="1"/>
+    <row r="782" s="4" customFormat="1"/>
+    <row r="783" s="4" customFormat="1"/>
+    <row r="784" s="4" customFormat="1"/>
+    <row r="785" s="4" customFormat="1"/>
+    <row r="786" s="4" customFormat="1"/>
+    <row r="787" s="4" customFormat="1"/>
+    <row r="788" s="4" customFormat="1"/>
+    <row r="789" s="4" customFormat="1"/>
+    <row r="790" s="4" customFormat="1"/>
+    <row r="791" s="4" customFormat="1"/>
+    <row r="792" s="4" customFormat="1"/>
+    <row r="793" s="4" customFormat="1"/>
+    <row r="794" s="4" customFormat="1"/>
+    <row r="795" s="4" customFormat="1"/>
+    <row r="796" s="4" customFormat="1"/>
+    <row r="797" s="4" customFormat="1"/>
+    <row r="798" s="4" customFormat="1"/>
+    <row r="799" s="4" customFormat="1"/>
+    <row r="800" s="4" customFormat="1"/>
+    <row r="801" s="4" customFormat="1"/>
+    <row r="802" s="4" customFormat="1"/>
+    <row r="803" s="4" customFormat="1"/>
+    <row r="804" s="4" customFormat="1"/>
+    <row r="805" s="4" customFormat="1"/>
+    <row r="806" s="4" customFormat="1"/>
+    <row r="807" s="4" customFormat="1"/>
+    <row r="808" s="4" customFormat="1"/>
+    <row r="809" s="4" customFormat="1"/>
+    <row r="810" s="4" customFormat="1"/>
+    <row r="811" s="4" customFormat="1"/>
+    <row r="812" s="4" customFormat="1"/>
+    <row r="813" s="4" customFormat="1"/>
+    <row r="814" s="4" customFormat="1"/>
+    <row r="815" s="4" customFormat="1"/>
+    <row r="816" s="4" customFormat="1"/>
+    <row r="817" s="4" customFormat="1"/>
+    <row r="818" s="4" customFormat="1"/>
+    <row r="819" s="4" customFormat="1"/>
+    <row r="820" s="4" customFormat="1"/>
+    <row r="821" s="4" customFormat="1"/>
+    <row r="822" s="4" customFormat="1"/>
+    <row r="823" s="4" customFormat="1"/>
+    <row r="824" s="4" customFormat="1"/>
+    <row r="825" s="4" customFormat="1"/>
+    <row r="826" s="4" customFormat="1"/>
+    <row r="827" s="4" customFormat="1"/>
+    <row r="828" s="4" customFormat="1"/>
+    <row r="829" s="4" customFormat="1"/>
+    <row r="830" s="4" customFormat="1"/>
+    <row r="831" s="4" customFormat="1"/>
+    <row r="832" s="4" customFormat="1"/>
+    <row r="833" s="4" customFormat="1"/>
+    <row r="834" s="4" customFormat="1"/>
+    <row r="835" s="4" customFormat="1"/>
+    <row r="836" s="4" customFormat="1"/>
+    <row r="837" s="4" customFormat="1"/>
+    <row r="838" s="4" customFormat="1"/>
+    <row r="839" s="4" customFormat="1"/>
+    <row r="840" s="4" customFormat="1"/>
+    <row r="841" s="4" customFormat="1"/>
+    <row r="842" s="4" customFormat="1"/>
+    <row r="843" s="4" customFormat="1"/>
+    <row r="844" s="4" customFormat="1"/>
+    <row r="845" s="4" customFormat="1"/>
+    <row r="846" s="4" customFormat="1"/>
+    <row r="847" s="4" customFormat="1"/>
+    <row r="848" s="4" customFormat="1"/>
+    <row r="849" s="4" customFormat="1"/>
+    <row r="850" s="4" customFormat="1"/>
+    <row r="851" s="4" customFormat="1"/>
+    <row r="852" s="4" customFormat="1"/>
+    <row r="853" s="4" customFormat="1"/>
+    <row r="854" s="4" customFormat="1"/>
+    <row r="855" s="4" customFormat="1"/>
+    <row r="856" s="4" customFormat="1"/>
+    <row r="857" s="4" customFormat="1"/>
+    <row r="858" s="4" customFormat="1"/>
+    <row r="859" s="4" customFormat="1"/>
+    <row r="860" s="4" customFormat="1"/>
+    <row r="861" s="4" customFormat="1"/>
+    <row r="862" s="4" customFormat="1"/>
+    <row r="863" s="4" customFormat="1"/>
+    <row r="864" s="4" customFormat="1"/>
+    <row r="865" s="4" customFormat="1"/>
+    <row r="866" s="4" customFormat="1"/>
+    <row r="867" s="4" customFormat="1"/>
+    <row r="868" s="4" customFormat="1"/>
+    <row r="869" s="4" customFormat="1"/>
+    <row r="870" s="4" customFormat="1"/>
+    <row r="871" s="4" customFormat="1"/>
+    <row r="872" s="4" customFormat="1"/>
+    <row r="873" s="4" customFormat="1"/>
+    <row r="874" s="4" customFormat="1"/>
+    <row r="875" s="4" customFormat="1"/>
+    <row r="876" s="4" customFormat="1"/>
+    <row r="877" s="4" customFormat="1"/>
+    <row r="878" s="4" customFormat="1"/>
+    <row r="879" s="4" customFormat="1"/>
+    <row r="880" s="4" customFormat="1"/>
+    <row r="881" s="4" customFormat="1"/>
+    <row r="882" s="4" customFormat="1"/>
+    <row r="883" s="4" customFormat="1"/>
+    <row r="884" s="4" customFormat="1"/>
+    <row r="885" s="4" customFormat="1"/>
+    <row r="886" s="4" customFormat="1"/>
+    <row r="887" s="4" customFormat="1"/>
+    <row r="888" s="4" customFormat="1"/>
+    <row r="889" s="4" customFormat="1"/>
+    <row r="890" s="4" customFormat="1"/>
+    <row r="891" s="4" customFormat="1"/>
+    <row r="892" s="4" customFormat="1"/>
+    <row r="893" s="4" customFormat="1"/>
+    <row r="894" s="4" customFormat="1"/>
+    <row r="895" s="4" customFormat="1"/>
+    <row r="896" s="4" customFormat="1"/>
+    <row r="897" s="4" customFormat="1"/>
+    <row r="898" s="4" customFormat="1"/>
+    <row r="899" s="4" customFormat="1"/>
+    <row r="900" s="4" customFormat="1"/>
+    <row r="901" s="4" customFormat="1"/>
+    <row r="902" s="4" customFormat="1"/>
+    <row r="903" s="4" customFormat="1"/>
+    <row r="904" s="4" customFormat="1"/>
+    <row r="905" s="4" customFormat="1"/>
+    <row r="906" s="4" customFormat="1"/>
+    <row r="907" s="4" customFormat="1"/>
+    <row r="908" s="4" customFormat="1"/>
+    <row r="909" s="4" customFormat="1"/>
+    <row r="910" s="4" customFormat="1"/>
+    <row r="911" s="4" customFormat="1"/>
+    <row r="912" s="4" customFormat="1"/>
+    <row r="913" s="4" customFormat="1"/>
+    <row r="914" s="4" customFormat="1"/>
+    <row r="915" s="4" customFormat="1"/>
+    <row r="916" s="4" customFormat="1"/>
+    <row r="917" s="4" customFormat="1"/>
+    <row r="918" s="4" customFormat="1"/>
+    <row r="919" s="4" customFormat="1"/>
+    <row r="920" s="4" customFormat="1"/>
+    <row r="921" s="4" customFormat="1"/>
+    <row r="922" s="4" customFormat="1"/>
+    <row r="923" s="4" customFormat="1"/>
+    <row r="924" s="4" customFormat="1"/>
+    <row r="925" s="4" customFormat="1"/>
+    <row r="926" s="4" customFormat="1"/>
+    <row r="927" s="4" customFormat="1"/>
+    <row r="928" s="4" customFormat="1"/>
+    <row r="929" s="4" customFormat="1"/>
+    <row r="930" s="4" customFormat="1"/>
+    <row r="931" s="4" customFormat="1"/>
+    <row r="932" s="4" customFormat="1"/>
+    <row r="933" s="4" customFormat="1"/>
+    <row r="934" s="4" customFormat="1"/>
+    <row r="935" s="4" customFormat="1"/>
+    <row r="936" s="4" customFormat="1"/>
+    <row r="937" s="4" customFormat="1"/>
+    <row r="938" s="4" customFormat="1"/>
+    <row r="939" s="4" customFormat="1"/>
+    <row r="940" s="4" customFormat="1"/>
+    <row r="941" s="4" customFormat="1"/>
+    <row r="942" s="4" customFormat="1"/>
+    <row r="943" s="4" customFormat="1"/>
+    <row r="944" s="4" customFormat="1"/>
+    <row r="945" s="4" customFormat="1"/>
+    <row r="946" s="4" customFormat="1"/>
+    <row r="947" s="4" customFormat="1"/>
+    <row r="948" s="4" customFormat="1"/>
+    <row r="949" s="4" customFormat="1"/>
+    <row r="950" s="4" customFormat="1"/>
+    <row r="951" s="4" customFormat="1"/>
+    <row r="952" s="4" customFormat="1"/>
+    <row r="953" s="4" customFormat="1"/>
+    <row r="954" s="4" customFormat="1"/>
+    <row r="955" s="4" customFormat="1"/>
+    <row r="956" s="4" customFormat="1"/>
+    <row r="957" s="4" customFormat="1"/>
+    <row r="958" s="4" customFormat="1"/>
+    <row r="959" s="4" customFormat="1"/>
+    <row r="960" s="4" customFormat="1"/>
+    <row r="961" s="4" customFormat="1"/>
+    <row r="962" s="4" customFormat="1"/>
+    <row r="963" s="4" customFormat="1"/>
+    <row r="964" s="4" customFormat="1"/>
+    <row r="965" s="4" customFormat="1"/>
+    <row r="966" s="4" customFormat="1"/>
+    <row r="967" s="4" customFormat="1"/>
+    <row r="968" s="4" customFormat="1"/>
+    <row r="969" s="4" customFormat="1"/>
+    <row r="970" s="4" customFormat="1"/>
+    <row r="971" s="4" customFormat="1"/>
+    <row r="972" s="4" customFormat="1"/>
+    <row r="973" s="4" customFormat="1"/>
+    <row r="974" s="4" customFormat="1"/>
+    <row r="975" s="4" customFormat="1"/>
+    <row r="976" s="4" customFormat="1"/>
+    <row r="977" s="4" customFormat="1"/>
+    <row r="978" s="4" customFormat="1"/>
+    <row r="979" s="4" customFormat="1"/>
+    <row r="980" s="4" customFormat="1"/>
+    <row r="981" s="4" customFormat="1"/>
+    <row r="982" s="4" customFormat="1"/>
+    <row r="983" s="4" customFormat="1"/>
+    <row r="984" s="4" customFormat="1"/>
+    <row r="985" s="4" customFormat="1"/>
+    <row r="986" s="4" customFormat="1"/>
+    <row r="987" s="4" customFormat="1"/>
+    <row r="988" s="4" customFormat="1"/>
+    <row r="989" s="4" customFormat="1"/>
+    <row r="990" s="4" customFormat="1"/>
+    <row r="991" s="4" customFormat="1"/>
+    <row r="992" s="4" customFormat="1"/>
+    <row r="993" s="4" customFormat="1"/>
+    <row r="994" s="4" customFormat="1"/>
+    <row r="995" s="4" customFormat="1"/>
+    <row r="996" s="4" customFormat="1"/>
+    <row r="997" s="4" customFormat="1"/>
+  </sheetData>
+  <phoneticPr fontId="2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Z987"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="41" customWidth="1"/>
+    <col min="2" max="2" width="51" customWidth="1"/>
+    <col min="3" max="3" width="75.3984375" customWidth="1"/>
+    <col min="4" max="26" width="8.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -545,1086 +1611,15 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="30">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
-    <row r="81" ht="14.25" customHeight="1"/>
-    <row r="82" ht="14.25" customHeight="1"/>
-    <row r="83" ht="14.25" customHeight="1"/>
-    <row r="84" ht="14.25" customHeight="1"/>
-    <row r="85" ht="14.25" customHeight="1"/>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
-    <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
-    <row r="91" ht="14.25" customHeight="1"/>
-    <row r="92" ht="14.25" customHeight="1"/>
-    <row r="93" ht="14.25" customHeight="1"/>
-    <row r="94" ht="14.25" customHeight="1"/>
-    <row r="95" ht="14.25" customHeight="1"/>
-    <row r="96" ht="14.25" customHeight="1"/>
-    <row r="97" ht="14.25" customHeight="1"/>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="14.25" customHeight="1"/>
-    <row r="101" ht="14.25" customHeight="1"/>
-    <row r="102" ht="14.25" customHeight="1"/>
-    <row r="103" ht="14.25" customHeight="1"/>
-    <row r="104" ht="14.25" customHeight="1"/>
-    <row r="105" ht="14.25" customHeight="1"/>
-    <row r="106" ht="14.25" customHeight="1"/>
-    <row r="107" ht="14.25" customHeight="1"/>
-    <row r="108" ht="14.25" customHeight="1"/>
-    <row r="109" ht="14.25" customHeight="1"/>
-    <row r="110" ht="14.25" customHeight="1"/>
-    <row r="111" ht="14.25" customHeight="1"/>
-    <row r="112" ht="14.25" customHeight="1"/>
-    <row r="113" ht="14.25" customHeight="1"/>
-    <row r="114" ht="14.25" customHeight="1"/>
-    <row r="115" ht="14.25" customHeight="1"/>
-    <row r="116" ht="14.25" customHeight="1"/>
-    <row r="117" ht="14.25" customHeight="1"/>
-    <row r="118" ht="14.25" customHeight="1"/>
-    <row r="119" ht="14.25" customHeight="1"/>
-    <row r="120" ht="14.25" customHeight="1"/>
-    <row r="121" ht="14.25" customHeight="1"/>
-    <row r="122" ht="14.25" customHeight="1"/>
-    <row r="123" ht="14.25" customHeight="1"/>
-    <row r="124" ht="14.25" customHeight="1"/>
-    <row r="125" ht="14.25" customHeight="1"/>
-    <row r="126" ht="14.25" customHeight="1"/>
-    <row r="127" ht="14.25" customHeight="1"/>
-    <row r="128" ht="14.25" customHeight="1"/>
-    <row r="129" ht="14.25" customHeight="1"/>
-    <row r="130" ht="14.25" customHeight="1"/>
-    <row r="131" ht="14.25" customHeight="1"/>
-    <row r="132" ht="14.25" customHeight="1"/>
-    <row r="133" ht="14.25" customHeight="1"/>
-    <row r="134" ht="14.25" customHeight="1"/>
-    <row r="135" ht="14.25" customHeight="1"/>
-    <row r="136" ht="14.25" customHeight="1"/>
-    <row r="137" ht="14.25" customHeight="1"/>
-    <row r="138" ht="14.25" customHeight="1"/>
-    <row r="139" ht="14.25" customHeight="1"/>
-    <row r="140" ht="14.25" customHeight="1"/>
-    <row r="141" ht="14.25" customHeight="1"/>
-    <row r="142" ht="14.25" customHeight="1"/>
-    <row r="143" ht="14.25" customHeight="1"/>
-    <row r="144" ht="14.25" customHeight="1"/>
-    <row r="145" ht="14.25" customHeight="1"/>
-    <row r="146" ht="14.25" customHeight="1"/>
-    <row r="147" ht="14.25" customHeight="1"/>
-    <row r="148" ht="14.25" customHeight="1"/>
-    <row r="149" ht="14.25" customHeight="1"/>
-    <row r="150" ht="14.25" customHeight="1"/>
-    <row r="151" ht="14.25" customHeight="1"/>
-    <row r="152" ht="14.25" customHeight="1"/>
-    <row r="153" ht="14.25" customHeight="1"/>
-    <row r="154" ht="14.25" customHeight="1"/>
-    <row r="155" ht="14.25" customHeight="1"/>
-    <row r="156" ht="14.25" customHeight="1"/>
-    <row r="157" ht="14.25" customHeight="1"/>
-    <row r="158" ht="14.25" customHeight="1"/>
-    <row r="159" ht="14.25" customHeight="1"/>
-    <row r="160" ht="14.25" customHeight="1"/>
-    <row r="161" ht="14.25" customHeight="1"/>
-    <row r="162" ht="14.25" customHeight="1"/>
-    <row r="163" ht="14.25" customHeight="1"/>
-    <row r="164" ht="14.25" customHeight="1"/>
-    <row r="165" ht="14.25" customHeight="1"/>
-    <row r="166" ht="14.25" customHeight="1"/>
-    <row r="167" ht="14.25" customHeight="1"/>
-    <row r="168" ht="14.25" customHeight="1"/>
-    <row r="169" ht="14.25" customHeight="1"/>
-    <row r="170" ht="14.25" customHeight="1"/>
-    <row r="171" ht="14.25" customHeight="1"/>
-    <row r="172" ht="14.25" customHeight="1"/>
-    <row r="173" ht="14.25" customHeight="1"/>
-    <row r="174" ht="14.25" customHeight="1"/>
-    <row r="175" ht="14.25" customHeight="1"/>
-    <row r="176" ht="14.25" customHeight="1"/>
-    <row r="177" ht="14.25" customHeight="1"/>
-    <row r="178" ht="14.25" customHeight="1"/>
-    <row r="179" ht="14.25" customHeight="1"/>
-    <row r="180" ht="14.25" customHeight="1"/>
-    <row r="181" ht="14.25" customHeight="1"/>
-    <row r="182" ht="14.25" customHeight="1"/>
-    <row r="183" ht="14.25" customHeight="1"/>
-    <row r="184" ht="14.25" customHeight="1"/>
-    <row r="185" ht="14.25" customHeight="1"/>
-    <row r="186" ht="14.25" customHeight="1"/>
-    <row r="187" ht="14.25" customHeight="1"/>
-    <row r="188" ht="14.25" customHeight="1"/>
-    <row r="189" ht="14.25" customHeight="1"/>
-    <row r="190" ht="14.25" customHeight="1"/>
-    <row r="191" ht="14.25" customHeight="1"/>
-    <row r="192" ht="14.25" customHeight="1"/>
-    <row r="193" ht="14.25" customHeight="1"/>
-    <row r="194" ht="14.25" customHeight="1"/>
-    <row r="195" ht="14.25" customHeight="1"/>
-    <row r="196" ht="14.25" customHeight="1"/>
-    <row r="197" ht="14.25" customHeight="1"/>
-    <row r="198" ht="14.25" customHeight="1"/>
-    <row r="199" ht="14.25" customHeight="1"/>
-    <row r="200" ht="14.25" customHeight="1"/>
-    <row r="201" ht="14.25" customHeight="1"/>
-    <row r="202" ht="14.25" customHeight="1"/>
-    <row r="203" ht="14.25" customHeight="1"/>
-    <row r="204" ht="14.25" customHeight="1"/>
-    <row r="205" ht="14.25" customHeight="1"/>
-    <row r="206" ht="14.25" customHeight="1"/>
-    <row r="207" ht="14.25" customHeight="1"/>
-    <row r="208" ht="14.25" customHeight="1"/>
-    <row r="209" ht="14.25" customHeight="1"/>
-    <row r="210" ht="14.25" customHeight="1"/>
-    <row r="211" ht="14.25" customHeight="1"/>
-    <row r="212" ht="14.25" customHeight="1"/>
-    <row r="213" ht="14.25" customHeight="1"/>
-    <row r="214" ht="14.25" customHeight="1"/>
-    <row r="215" ht="14.25" customHeight="1"/>
-    <row r="216" ht="14.25" customHeight="1"/>
-    <row r="217" ht="14.25" customHeight="1"/>
-    <row r="218" ht="14.25" customHeight="1"/>
-    <row r="219" ht="14.25" customHeight="1"/>
-    <row r="220" ht="14.25" customHeight="1"/>
-    <row r="221" ht="14.25" customHeight="1"/>
-    <row r="222" ht="14.25" customHeight="1"/>
-    <row r="223" ht="14.25" customHeight="1"/>
-    <row r="224" ht="14.25" customHeight="1"/>
-    <row r="225" ht="14.25" customHeight="1"/>
-    <row r="226" ht="14.25" customHeight="1"/>
-    <row r="227" ht="14.25" customHeight="1"/>
-    <row r="228" ht="14.25" customHeight="1"/>
-    <row r="229" ht="14.25" customHeight="1"/>
-    <row r="230" ht="14.25" customHeight="1"/>
-    <row r="231" ht="14.25" customHeight="1"/>
-    <row r="232" ht="14.25" customHeight="1"/>
-    <row r="233" ht="14.25" customHeight="1"/>
-    <row r="234" ht="14.25" customHeight="1"/>
-    <row r="235" ht="14.25" customHeight="1"/>
-    <row r="236" ht="14.25" customHeight="1"/>
-    <row r="237" ht="14.25" customHeight="1"/>
-    <row r="238" ht="14.25" customHeight="1"/>
-    <row r="239" ht="14.25" customHeight="1"/>
-    <row r="240" ht="14.25" customHeight="1"/>
-    <row r="241" ht="14.25" customHeight="1"/>
-    <row r="242" ht="14.25" customHeight="1"/>
-    <row r="243" ht="14.25" customHeight="1"/>
-    <row r="244" ht="14.25" customHeight="1"/>
-    <row r="245" ht="14.25" customHeight="1"/>
-    <row r="246" ht="14.25" customHeight="1"/>
-    <row r="247" ht="14.25" customHeight="1"/>
-    <row r="248" ht="14.25" customHeight="1"/>
-    <row r="249" ht="14.25" customHeight="1"/>
-    <row r="250" ht="14.25" customHeight="1"/>
-    <row r="251" ht="14.25" customHeight="1"/>
-    <row r="252" ht="14.25" customHeight="1"/>
-    <row r="253" ht="14.25" customHeight="1"/>
-    <row r="254" ht="14.25" customHeight="1"/>
-    <row r="255" ht="14.25" customHeight="1"/>
-    <row r="256" ht="14.25" customHeight="1"/>
-    <row r="257" ht="14.25" customHeight="1"/>
-    <row r="258" ht="14.25" customHeight="1"/>
-    <row r="259" ht="14.25" customHeight="1"/>
-    <row r="260" ht="14.25" customHeight="1"/>
-    <row r="261" ht="14.25" customHeight="1"/>
-    <row r="262" ht="14.25" customHeight="1"/>
-    <row r="263" ht="14.25" customHeight="1"/>
-    <row r="264" ht="14.25" customHeight="1"/>
-    <row r="265" ht="14.25" customHeight="1"/>
-    <row r="266" ht="14.25" customHeight="1"/>
-    <row r="267" ht="14.25" customHeight="1"/>
-    <row r="268" ht="14.25" customHeight="1"/>
-    <row r="269" ht="14.25" customHeight="1"/>
-    <row r="270" ht="14.25" customHeight="1"/>
-    <row r="271" ht="14.25" customHeight="1"/>
-    <row r="272" ht="14.25" customHeight="1"/>
-    <row r="273" ht="14.25" customHeight="1"/>
-    <row r="274" ht="14.25" customHeight="1"/>
-    <row r="275" ht="14.25" customHeight="1"/>
-    <row r="276" ht="14.25" customHeight="1"/>
-    <row r="277" ht="14.25" customHeight="1"/>
-    <row r="278" ht="14.25" customHeight="1"/>
-    <row r="279" ht="14.25" customHeight="1"/>
-    <row r="280" ht="14.25" customHeight="1"/>
-    <row r="281" ht="14.25" customHeight="1"/>
-    <row r="282" ht="14.25" customHeight="1"/>
-    <row r="283" ht="14.25" customHeight="1"/>
-    <row r="284" ht="14.25" customHeight="1"/>
-    <row r="285" ht="14.25" customHeight="1"/>
-    <row r="286" ht="14.25" customHeight="1"/>
-    <row r="287" ht="14.25" customHeight="1"/>
-    <row r="288" ht="14.25" customHeight="1"/>
-    <row r="289" ht="14.25" customHeight="1"/>
-    <row r="290" ht="14.25" customHeight="1"/>
-    <row r="291" ht="14.25" customHeight="1"/>
-    <row r="292" ht="14.25" customHeight="1"/>
-    <row r="293" ht="14.25" customHeight="1"/>
-    <row r="294" ht="14.25" customHeight="1"/>
-    <row r="295" ht="14.25" customHeight="1"/>
-    <row r="296" ht="14.25" customHeight="1"/>
-    <row r="297" ht="14.25" customHeight="1"/>
-    <row r="298" ht="14.25" customHeight="1"/>
-    <row r="299" ht="14.25" customHeight="1"/>
-    <row r="300" ht="14.25" customHeight="1"/>
-    <row r="301" ht="14.25" customHeight="1"/>
-    <row r="302" ht="14.25" customHeight="1"/>
-    <row r="303" ht="14.25" customHeight="1"/>
-    <row r="304" ht="14.25" customHeight="1"/>
-    <row r="305" ht="14.25" customHeight="1"/>
-    <row r="306" ht="14.25" customHeight="1"/>
-    <row r="307" ht="14.25" customHeight="1"/>
-    <row r="308" ht="14.25" customHeight="1"/>
-    <row r="309" ht="14.25" customHeight="1"/>
-    <row r="310" ht="14.25" customHeight="1"/>
-    <row r="311" ht="14.25" customHeight="1"/>
-    <row r="312" ht="14.25" customHeight="1"/>
-    <row r="313" ht="14.25" customHeight="1"/>
-    <row r="314" ht="14.25" customHeight="1"/>
-    <row r="315" ht="14.25" customHeight="1"/>
-    <row r="316" ht="14.25" customHeight="1"/>
-    <row r="317" ht="14.25" customHeight="1"/>
-    <row r="318" ht="14.25" customHeight="1"/>
-    <row r="319" ht="14.25" customHeight="1"/>
-    <row r="320" ht="14.25" customHeight="1"/>
-    <row r="321" ht="14.25" customHeight="1"/>
-    <row r="322" ht="14.25" customHeight="1"/>
-    <row r="323" ht="14.25" customHeight="1"/>
-    <row r="324" ht="14.25" customHeight="1"/>
-    <row r="325" ht="14.25" customHeight="1"/>
-    <row r="326" ht="14.25" customHeight="1"/>
-    <row r="327" ht="14.25" customHeight="1"/>
-    <row r="328" ht="14.25" customHeight="1"/>
-    <row r="329" ht="14.25" customHeight="1"/>
-    <row r="330" ht="14.25" customHeight="1"/>
-    <row r="331" ht="14.25" customHeight="1"/>
-    <row r="332" ht="14.25" customHeight="1"/>
-    <row r="333" ht="14.25" customHeight="1"/>
-    <row r="334" ht="14.25" customHeight="1"/>
-    <row r="335" ht="14.25" customHeight="1"/>
-    <row r="336" ht="14.25" customHeight="1"/>
-    <row r="337" ht="14.25" customHeight="1"/>
-    <row r="338" ht="14.25" customHeight="1"/>
-    <row r="339" ht="14.25" customHeight="1"/>
-    <row r="340" ht="14.25" customHeight="1"/>
-    <row r="341" ht="14.25" customHeight="1"/>
-    <row r="342" ht="14.25" customHeight="1"/>
-    <row r="343" ht="14.25" customHeight="1"/>
-    <row r="344" ht="14.25" customHeight="1"/>
-    <row r="345" ht="14.25" customHeight="1"/>
-    <row r="346" ht="14.25" customHeight="1"/>
-    <row r="347" ht="14.25" customHeight="1"/>
-    <row r="348" ht="14.25" customHeight="1"/>
-    <row r="349" ht="14.25" customHeight="1"/>
-    <row r="350" ht="14.25" customHeight="1"/>
-    <row r="351" ht="14.25" customHeight="1"/>
-    <row r="352" ht="14.25" customHeight="1"/>
-    <row r="353" ht="14.25" customHeight="1"/>
-    <row r="354" ht="14.25" customHeight="1"/>
-    <row r="355" ht="14.25" customHeight="1"/>
-    <row r="356" ht="14.25" customHeight="1"/>
-    <row r="357" ht="14.25" customHeight="1"/>
-    <row r="358" ht="14.25" customHeight="1"/>
-    <row r="359" ht="14.25" customHeight="1"/>
-    <row r="360" ht="14.25" customHeight="1"/>
-    <row r="361" ht="14.25" customHeight="1"/>
-    <row r="362" ht="14.25" customHeight="1"/>
-    <row r="363" ht="14.25" customHeight="1"/>
-    <row r="364" ht="14.25" customHeight="1"/>
-    <row r="365" ht="14.25" customHeight="1"/>
-    <row r="366" ht="14.25" customHeight="1"/>
-    <row r="367" ht="14.25" customHeight="1"/>
-    <row r="368" ht="14.25" customHeight="1"/>
-    <row r="369" ht="14.25" customHeight="1"/>
-    <row r="370" ht="14.25" customHeight="1"/>
-    <row r="371" ht="14.25" customHeight="1"/>
-    <row r="372" ht="14.25" customHeight="1"/>
-    <row r="373" ht="14.25" customHeight="1"/>
-    <row r="374" ht="14.25" customHeight="1"/>
-    <row r="375" ht="14.25" customHeight="1"/>
-    <row r="376" ht="14.25" customHeight="1"/>
-    <row r="377" ht="14.25" customHeight="1"/>
-    <row r="378" ht="14.25" customHeight="1"/>
-    <row r="379" ht="14.25" customHeight="1"/>
-    <row r="380" ht="14.25" customHeight="1"/>
-    <row r="381" ht="14.25" customHeight="1"/>
-    <row r="382" ht="14.25" customHeight="1"/>
-    <row r="383" ht="14.25" customHeight="1"/>
-    <row r="384" ht="14.25" customHeight="1"/>
-    <row r="385" ht="14.25" customHeight="1"/>
-    <row r="386" ht="14.25" customHeight="1"/>
-    <row r="387" ht="14.25" customHeight="1"/>
-    <row r="388" ht="14.25" customHeight="1"/>
-    <row r="389" ht="14.25" customHeight="1"/>
-    <row r="390" ht="14.25" customHeight="1"/>
-    <row r="391" ht="14.25" customHeight="1"/>
-    <row r="392" ht="14.25" customHeight="1"/>
-    <row r="393" ht="14.25" customHeight="1"/>
-    <row r="394" ht="14.25" customHeight="1"/>
-    <row r="395" ht="14.25" customHeight="1"/>
-    <row r="396" ht="14.25" customHeight="1"/>
-    <row r="397" ht="14.25" customHeight="1"/>
-    <row r="398" ht="14.25" customHeight="1"/>
-    <row r="399" ht="14.25" customHeight="1"/>
-    <row r="400" ht="14.25" customHeight="1"/>
-    <row r="401" ht="14.25" customHeight="1"/>
-    <row r="402" ht="14.25" customHeight="1"/>
-    <row r="403" ht="14.25" customHeight="1"/>
-    <row r="404" ht="14.25" customHeight="1"/>
-    <row r="405" ht="14.25" customHeight="1"/>
-    <row r="406" ht="14.25" customHeight="1"/>
-    <row r="407" ht="14.25" customHeight="1"/>
-    <row r="408" ht="14.25" customHeight="1"/>
-    <row r="409" ht="14.25" customHeight="1"/>
-    <row r="410" ht="14.25" customHeight="1"/>
-    <row r="411" ht="14.25" customHeight="1"/>
-    <row r="412" ht="14.25" customHeight="1"/>
-    <row r="413" ht="14.25" customHeight="1"/>
-    <row r="414" ht="14.25" customHeight="1"/>
-    <row r="415" ht="14.25" customHeight="1"/>
-    <row r="416" ht="14.25" customHeight="1"/>
-    <row r="417" ht="14.25" customHeight="1"/>
-    <row r="418" ht="14.25" customHeight="1"/>
-    <row r="419" ht="14.25" customHeight="1"/>
-    <row r="420" ht="14.25" customHeight="1"/>
-    <row r="421" ht="14.25" customHeight="1"/>
-    <row r="422" ht="14.25" customHeight="1"/>
-    <row r="423" ht="14.25" customHeight="1"/>
-    <row r="424" ht="14.25" customHeight="1"/>
-    <row r="425" ht="14.25" customHeight="1"/>
-    <row r="426" ht="14.25" customHeight="1"/>
-    <row r="427" ht="14.25" customHeight="1"/>
-    <row r="428" ht="14.25" customHeight="1"/>
-    <row r="429" ht="14.25" customHeight="1"/>
-    <row r="430" ht="14.25" customHeight="1"/>
-    <row r="431" ht="14.25" customHeight="1"/>
-    <row r="432" ht="14.25" customHeight="1"/>
-    <row r="433" ht="14.25" customHeight="1"/>
-    <row r="434" ht="14.25" customHeight="1"/>
-    <row r="435" ht="14.25" customHeight="1"/>
-    <row r="436" ht="14.25" customHeight="1"/>
-    <row r="437" ht="14.25" customHeight="1"/>
-    <row r="438" ht="14.25" customHeight="1"/>
-    <row r="439" ht="14.25" customHeight="1"/>
-    <row r="440" ht="14.25" customHeight="1"/>
-    <row r="441" ht="14.25" customHeight="1"/>
-    <row r="442" ht="14.25" customHeight="1"/>
-    <row r="443" ht="14.25" customHeight="1"/>
-    <row r="444" ht="14.25" customHeight="1"/>
-    <row r="445" ht="14.25" customHeight="1"/>
-    <row r="446" ht="14.25" customHeight="1"/>
-    <row r="447" ht="14.25" customHeight="1"/>
-    <row r="448" ht="14.25" customHeight="1"/>
-    <row r="449" ht="14.25" customHeight="1"/>
-    <row r="450" ht="14.25" customHeight="1"/>
-    <row r="451" ht="14.25" customHeight="1"/>
-    <row r="452" ht="14.25" customHeight="1"/>
-    <row r="453" ht="14.25" customHeight="1"/>
-    <row r="454" ht="14.25" customHeight="1"/>
-    <row r="455" ht="14.25" customHeight="1"/>
-    <row r="456" ht="14.25" customHeight="1"/>
-    <row r="457" ht="14.25" customHeight="1"/>
-    <row r="458" ht="14.25" customHeight="1"/>
-    <row r="459" ht="14.25" customHeight="1"/>
-    <row r="460" ht="14.25" customHeight="1"/>
-    <row r="461" ht="14.25" customHeight="1"/>
-    <row r="462" ht="14.25" customHeight="1"/>
-    <row r="463" ht="14.25" customHeight="1"/>
-    <row r="464" ht="14.25" customHeight="1"/>
-    <row r="465" ht="14.25" customHeight="1"/>
-    <row r="466" ht="14.25" customHeight="1"/>
-    <row r="467" ht="14.25" customHeight="1"/>
-    <row r="468" ht="14.25" customHeight="1"/>
-    <row r="469" ht="14.25" customHeight="1"/>
-    <row r="470" ht="14.25" customHeight="1"/>
-    <row r="471" ht="14.25" customHeight="1"/>
-    <row r="472" ht="14.25" customHeight="1"/>
-    <row r="473" ht="14.25" customHeight="1"/>
-    <row r="474" ht="14.25" customHeight="1"/>
-    <row r="475" ht="14.25" customHeight="1"/>
-    <row r="476" ht="14.25" customHeight="1"/>
-    <row r="477" ht="14.25" customHeight="1"/>
-    <row r="478" ht="14.25" customHeight="1"/>
-    <row r="479" ht="14.25" customHeight="1"/>
-    <row r="480" ht="14.25" customHeight="1"/>
-    <row r="481" ht="14.25" customHeight="1"/>
-    <row r="482" ht="14.25" customHeight="1"/>
-    <row r="483" ht="14.25" customHeight="1"/>
-    <row r="484" ht="14.25" customHeight="1"/>
-    <row r="485" ht="14.25" customHeight="1"/>
-    <row r="486" ht="14.25" customHeight="1"/>
-    <row r="487" ht="14.25" customHeight="1"/>
-    <row r="488" ht="14.25" customHeight="1"/>
-    <row r="489" ht="14.25" customHeight="1"/>
-    <row r="490" ht="14.25" customHeight="1"/>
-    <row r="491" ht="14.25" customHeight="1"/>
-    <row r="492" ht="14.25" customHeight="1"/>
-    <row r="493" ht="14.25" customHeight="1"/>
-    <row r="494" ht="14.25" customHeight="1"/>
-    <row r="495" ht="14.25" customHeight="1"/>
-    <row r="496" ht="14.25" customHeight="1"/>
-    <row r="497" ht="14.25" customHeight="1"/>
-    <row r="498" ht="14.25" customHeight="1"/>
-    <row r="499" ht="14.25" customHeight="1"/>
-    <row r="500" ht="14.25" customHeight="1"/>
-    <row r="501" ht="14.25" customHeight="1"/>
-    <row r="502" ht="14.25" customHeight="1"/>
-    <row r="503" ht="14.25" customHeight="1"/>
-    <row r="504" ht="14.25" customHeight="1"/>
-    <row r="505" ht="14.25" customHeight="1"/>
-    <row r="506" ht="14.25" customHeight="1"/>
-    <row r="507" ht="14.25" customHeight="1"/>
-    <row r="508" ht="14.25" customHeight="1"/>
-    <row r="509" ht="14.25" customHeight="1"/>
-    <row r="510" ht="14.25" customHeight="1"/>
-    <row r="511" ht="14.25" customHeight="1"/>
-    <row r="512" ht="14.25" customHeight="1"/>
-    <row r="513" ht="14.25" customHeight="1"/>
-    <row r="514" ht="14.25" customHeight="1"/>
-    <row r="515" ht="14.25" customHeight="1"/>
-    <row r="516" ht="14.25" customHeight="1"/>
-    <row r="517" ht="14.25" customHeight="1"/>
-    <row r="518" ht="14.25" customHeight="1"/>
-    <row r="519" ht="14.25" customHeight="1"/>
-    <row r="520" ht="14.25" customHeight="1"/>
-    <row r="521" ht="14.25" customHeight="1"/>
-    <row r="522" ht="14.25" customHeight="1"/>
-    <row r="523" ht="14.25" customHeight="1"/>
-    <row r="524" ht="14.25" customHeight="1"/>
-    <row r="525" ht="14.25" customHeight="1"/>
-    <row r="526" ht="14.25" customHeight="1"/>
-    <row r="527" ht="14.25" customHeight="1"/>
-    <row r="528" ht="14.25" customHeight="1"/>
-    <row r="529" ht="14.25" customHeight="1"/>
-    <row r="530" ht="14.25" customHeight="1"/>
-    <row r="531" ht="14.25" customHeight="1"/>
-    <row r="532" ht="14.25" customHeight="1"/>
-    <row r="533" ht="14.25" customHeight="1"/>
-    <row r="534" ht="14.25" customHeight="1"/>
-    <row r="535" ht="14.25" customHeight="1"/>
-    <row r="536" ht="14.25" customHeight="1"/>
-    <row r="537" ht="14.25" customHeight="1"/>
-    <row r="538" ht="14.25" customHeight="1"/>
-    <row r="539" ht="14.25" customHeight="1"/>
-    <row r="540" ht="14.25" customHeight="1"/>
-    <row r="541" ht="14.25" customHeight="1"/>
-    <row r="542" ht="14.25" customHeight="1"/>
-    <row r="543" ht="14.25" customHeight="1"/>
-    <row r="544" ht="14.25" customHeight="1"/>
-    <row r="545" ht="14.25" customHeight="1"/>
-    <row r="546" ht="14.25" customHeight="1"/>
-    <row r="547" ht="14.25" customHeight="1"/>
-    <row r="548" ht="14.25" customHeight="1"/>
-    <row r="549" ht="14.25" customHeight="1"/>
-    <row r="550" ht="14.25" customHeight="1"/>
-    <row r="551" ht="14.25" customHeight="1"/>
-    <row r="552" ht="14.25" customHeight="1"/>
-    <row r="553" ht="14.25" customHeight="1"/>
-    <row r="554" ht="14.25" customHeight="1"/>
-    <row r="555" ht="14.25" customHeight="1"/>
-    <row r="556" ht="14.25" customHeight="1"/>
-    <row r="557" ht="14.25" customHeight="1"/>
-    <row r="558" ht="14.25" customHeight="1"/>
-    <row r="559" ht="14.25" customHeight="1"/>
-    <row r="560" ht="14.25" customHeight="1"/>
-    <row r="561" ht="14.25" customHeight="1"/>
-    <row r="562" ht="14.25" customHeight="1"/>
-    <row r="563" ht="14.25" customHeight="1"/>
-    <row r="564" ht="14.25" customHeight="1"/>
-    <row r="565" ht="14.25" customHeight="1"/>
-    <row r="566" ht="14.25" customHeight="1"/>
-    <row r="567" ht="14.25" customHeight="1"/>
-    <row r="568" ht="14.25" customHeight="1"/>
-    <row r="569" ht="14.25" customHeight="1"/>
-    <row r="570" ht="14.25" customHeight="1"/>
-    <row r="571" ht="14.25" customHeight="1"/>
-    <row r="572" ht="14.25" customHeight="1"/>
-    <row r="573" ht="14.25" customHeight="1"/>
-    <row r="574" ht="14.25" customHeight="1"/>
-    <row r="575" ht="14.25" customHeight="1"/>
-    <row r="576" ht="14.25" customHeight="1"/>
-    <row r="577" ht="14.25" customHeight="1"/>
-    <row r="578" ht="14.25" customHeight="1"/>
-    <row r="579" ht="14.25" customHeight="1"/>
-    <row r="580" ht="14.25" customHeight="1"/>
-    <row r="581" ht="14.25" customHeight="1"/>
-    <row r="582" ht="14.25" customHeight="1"/>
-    <row r="583" ht="14.25" customHeight="1"/>
-    <row r="584" ht="14.25" customHeight="1"/>
-    <row r="585" ht="14.25" customHeight="1"/>
-    <row r="586" ht="14.25" customHeight="1"/>
-    <row r="587" ht="14.25" customHeight="1"/>
-    <row r="588" ht="14.25" customHeight="1"/>
-    <row r="589" ht="14.25" customHeight="1"/>
-    <row r="590" ht="14.25" customHeight="1"/>
-    <row r="591" ht="14.25" customHeight="1"/>
-    <row r="592" ht="14.25" customHeight="1"/>
-    <row r="593" ht="14.25" customHeight="1"/>
-    <row r="594" ht="14.25" customHeight="1"/>
-    <row r="595" ht="14.25" customHeight="1"/>
-    <row r="596" ht="14.25" customHeight="1"/>
-    <row r="597" ht="14.25" customHeight="1"/>
-    <row r="598" ht="14.25" customHeight="1"/>
-    <row r="599" ht="14.25" customHeight="1"/>
-    <row r="600" ht="14.25" customHeight="1"/>
-    <row r="601" ht="14.25" customHeight="1"/>
-    <row r="602" ht="14.25" customHeight="1"/>
-    <row r="603" ht="14.25" customHeight="1"/>
-    <row r="604" ht="14.25" customHeight="1"/>
-    <row r="605" ht="14.25" customHeight="1"/>
-    <row r="606" ht="14.25" customHeight="1"/>
-    <row r="607" ht="14.25" customHeight="1"/>
-    <row r="608" ht="14.25" customHeight="1"/>
-    <row r="609" ht="14.25" customHeight="1"/>
-    <row r="610" ht="14.25" customHeight="1"/>
-    <row r="611" ht="14.25" customHeight="1"/>
-    <row r="612" ht="14.25" customHeight="1"/>
-    <row r="613" ht="14.25" customHeight="1"/>
-    <row r="614" ht="14.25" customHeight="1"/>
-    <row r="615" ht="14.25" customHeight="1"/>
-    <row r="616" ht="14.25" customHeight="1"/>
-    <row r="617" ht="14.25" customHeight="1"/>
-    <row r="618" ht="14.25" customHeight="1"/>
-    <row r="619" ht="14.25" customHeight="1"/>
-    <row r="620" ht="14.25" customHeight="1"/>
-    <row r="621" ht="14.25" customHeight="1"/>
-    <row r="622" ht="14.25" customHeight="1"/>
-    <row r="623" ht="14.25" customHeight="1"/>
-    <row r="624" ht="14.25" customHeight="1"/>
-    <row r="625" ht="14.25" customHeight="1"/>
-    <row r="626" ht="14.25" customHeight="1"/>
-    <row r="627" ht="14.25" customHeight="1"/>
-    <row r="628" ht="14.25" customHeight="1"/>
-    <row r="629" ht="14.25" customHeight="1"/>
-    <row r="630" ht="14.25" customHeight="1"/>
-    <row r="631" ht="14.25" customHeight="1"/>
-    <row r="632" ht="14.25" customHeight="1"/>
-    <row r="633" ht="14.25" customHeight="1"/>
-    <row r="634" ht="14.25" customHeight="1"/>
-    <row r="635" ht="14.25" customHeight="1"/>
-    <row r="636" ht="14.25" customHeight="1"/>
-    <row r="637" ht="14.25" customHeight="1"/>
-    <row r="638" ht="14.25" customHeight="1"/>
-    <row r="639" ht="14.25" customHeight="1"/>
-    <row r="640" ht="14.25" customHeight="1"/>
-    <row r="641" ht="14.25" customHeight="1"/>
-    <row r="642" ht="14.25" customHeight="1"/>
-    <row r="643" ht="14.25" customHeight="1"/>
-    <row r="644" ht="14.25" customHeight="1"/>
-    <row r="645" ht="14.25" customHeight="1"/>
-    <row r="646" ht="14.25" customHeight="1"/>
-    <row r="647" ht="14.25" customHeight="1"/>
-    <row r="648" ht="14.25" customHeight="1"/>
-    <row r="649" ht="14.25" customHeight="1"/>
-    <row r="650" ht="14.25" customHeight="1"/>
-    <row r="651" ht="14.25" customHeight="1"/>
-    <row r="652" ht="14.25" customHeight="1"/>
-    <row r="653" ht="14.25" customHeight="1"/>
-    <row r="654" ht="14.25" customHeight="1"/>
-    <row r="655" ht="14.25" customHeight="1"/>
-    <row r="656" ht="14.25" customHeight="1"/>
-    <row r="657" ht="14.25" customHeight="1"/>
-    <row r="658" ht="14.25" customHeight="1"/>
-    <row r="659" ht="14.25" customHeight="1"/>
-    <row r="660" ht="14.25" customHeight="1"/>
-    <row r="661" ht="14.25" customHeight="1"/>
-    <row r="662" ht="14.25" customHeight="1"/>
-    <row r="663" ht="14.25" customHeight="1"/>
-    <row r="664" ht="14.25" customHeight="1"/>
-    <row r="665" ht="14.25" customHeight="1"/>
-    <row r="666" ht="14.25" customHeight="1"/>
-    <row r="667" ht="14.25" customHeight="1"/>
-    <row r="668" ht="14.25" customHeight="1"/>
-    <row r="669" ht="14.25" customHeight="1"/>
-    <row r="670" ht="14.25" customHeight="1"/>
-    <row r="671" ht="14.25" customHeight="1"/>
-    <row r="672" ht="14.25" customHeight="1"/>
-    <row r="673" ht="14.25" customHeight="1"/>
-    <row r="674" ht="14.25" customHeight="1"/>
-    <row r="675" ht="14.25" customHeight="1"/>
-    <row r="676" ht="14.25" customHeight="1"/>
-    <row r="677" ht="14.25" customHeight="1"/>
-    <row r="678" ht="14.25" customHeight="1"/>
-    <row r="679" ht="14.25" customHeight="1"/>
-    <row r="680" ht="14.25" customHeight="1"/>
-    <row r="681" ht="14.25" customHeight="1"/>
-    <row r="682" ht="14.25" customHeight="1"/>
-    <row r="683" ht="14.25" customHeight="1"/>
-    <row r="684" ht="14.25" customHeight="1"/>
-    <row r="685" ht="14.25" customHeight="1"/>
-    <row r="686" ht="14.25" customHeight="1"/>
-    <row r="687" ht="14.25" customHeight="1"/>
-    <row r="688" ht="14.25" customHeight="1"/>
-    <row r="689" ht="14.25" customHeight="1"/>
-    <row r="690" ht="14.25" customHeight="1"/>
-    <row r="691" ht="14.25" customHeight="1"/>
-    <row r="692" ht="14.25" customHeight="1"/>
-    <row r="693" ht="14.25" customHeight="1"/>
-    <row r="694" ht="14.25" customHeight="1"/>
-    <row r="695" ht="14.25" customHeight="1"/>
-    <row r="696" ht="14.25" customHeight="1"/>
-    <row r="697" ht="14.25" customHeight="1"/>
-    <row r="698" ht="14.25" customHeight="1"/>
-    <row r="699" ht="14.25" customHeight="1"/>
-    <row r="700" ht="14.25" customHeight="1"/>
-    <row r="701" ht="14.25" customHeight="1"/>
-    <row r="702" ht="14.25" customHeight="1"/>
-    <row r="703" ht="14.25" customHeight="1"/>
-    <row r="704" ht="14.25" customHeight="1"/>
-    <row r="705" ht="14.25" customHeight="1"/>
-    <row r="706" ht="14.25" customHeight="1"/>
-    <row r="707" ht="14.25" customHeight="1"/>
-    <row r="708" ht="14.25" customHeight="1"/>
-    <row r="709" ht="14.25" customHeight="1"/>
-    <row r="710" ht="14.25" customHeight="1"/>
-    <row r="711" ht="14.25" customHeight="1"/>
-    <row r="712" ht="14.25" customHeight="1"/>
-    <row r="713" ht="14.25" customHeight="1"/>
-    <row r="714" ht="14.25" customHeight="1"/>
-    <row r="715" ht="14.25" customHeight="1"/>
-    <row r="716" ht="14.25" customHeight="1"/>
-    <row r="717" ht="14.25" customHeight="1"/>
-    <row r="718" ht="14.25" customHeight="1"/>
-    <row r="719" ht="14.25" customHeight="1"/>
-    <row r="720" ht="14.25" customHeight="1"/>
-    <row r="721" ht="14.25" customHeight="1"/>
-    <row r="722" ht="14.25" customHeight="1"/>
-    <row r="723" ht="14.25" customHeight="1"/>
-    <row r="724" ht="14.25" customHeight="1"/>
-    <row r="725" ht="14.25" customHeight="1"/>
-    <row r="726" ht="14.25" customHeight="1"/>
-    <row r="727" ht="14.25" customHeight="1"/>
-    <row r="728" ht="14.25" customHeight="1"/>
-    <row r="729" ht="14.25" customHeight="1"/>
-    <row r="730" ht="14.25" customHeight="1"/>
-    <row r="731" ht="14.25" customHeight="1"/>
-    <row r="732" ht="14.25" customHeight="1"/>
-    <row r="733" ht="14.25" customHeight="1"/>
-    <row r="734" ht="14.25" customHeight="1"/>
-    <row r="735" ht="14.25" customHeight="1"/>
-    <row r="736" ht="14.25" customHeight="1"/>
-    <row r="737" ht="14.25" customHeight="1"/>
-    <row r="738" ht="14.25" customHeight="1"/>
-    <row r="739" ht="14.25" customHeight="1"/>
-    <row r="740" ht="14.25" customHeight="1"/>
-    <row r="741" ht="14.25" customHeight="1"/>
-    <row r="742" ht="14.25" customHeight="1"/>
-    <row r="743" ht="14.25" customHeight="1"/>
-    <row r="744" ht="14.25" customHeight="1"/>
-    <row r="745" ht="14.25" customHeight="1"/>
-    <row r="746" ht="14.25" customHeight="1"/>
-    <row r="747" ht="14.25" customHeight="1"/>
-    <row r="748" ht="14.25" customHeight="1"/>
-    <row r="749" ht="14.25" customHeight="1"/>
-    <row r="750" ht="14.25" customHeight="1"/>
-    <row r="751" ht="14.25" customHeight="1"/>
-    <row r="752" ht="14.25" customHeight="1"/>
-    <row r="753" ht="14.25" customHeight="1"/>
-    <row r="754" ht="14.25" customHeight="1"/>
-    <row r="755" ht="14.25" customHeight="1"/>
-    <row r="756" ht="14.25" customHeight="1"/>
-    <row r="757" ht="14.25" customHeight="1"/>
-    <row r="758" ht="14.25" customHeight="1"/>
-    <row r="759" ht="14.25" customHeight="1"/>
-    <row r="760" ht="14.25" customHeight="1"/>
-    <row r="761" ht="14.25" customHeight="1"/>
-    <row r="762" ht="14.25" customHeight="1"/>
-    <row r="763" ht="14.25" customHeight="1"/>
-    <row r="764" ht="14.25" customHeight="1"/>
-    <row r="765" ht="14.25" customHeight="1"/>
-    <row r="766" ht="14.25" customHeight="1"/>
-    <row r="767" ht="14.25" customHeight="1"/>
-    <row r="768" ht="14.25" customHeight="1"/>
-    <row r="769" ht="14.25" customHeight="1"/>
-    <row r="770" ht="14.25" customHeight="1"/>
-    <row r="771" ht="14.25" customHeight="1"/>
-    <row r="772" ht="14.25" customHeight="1"/>
-    <row r="773" ht="14.25" customHeight="1"/>
-    <row r="774" ht="14.25" customHeight="1"/>
-    <row r="775" ht="14.25" customHeight="1"/>
-    <row r="776" ht="14.25" customHeight="1"/>
-    <row r="777" ht="14.25" customHeight="1"/>
-    <row r="778" ht="14.25" customHeight="1"/>
-    <row r="779" ht="14.25" customHeight="1"/>
-    <row r="780" ht="14.25" customHeight="1"/>
-    <row r="781" ht="14.25" customHeight="1"/>
-    <row r="782" ht="14.25" customHeight="1"/>
-    <row r="783" ht="14.25" customHeight="1"/>
-    <row r="784" ht="14.25" customHeight="1"/>
-    <row r="785" ht="14.25" customHeight="1"/>
-    <row r="786" ht="14.25" customHeight="1"/>
-    <row r="787" ht="14.25" customHeight="1"/>
-    <row r="788" ht="14.25" customHeight="1"/>
-    <row r="789" ht="14.25" customHeight="1"/>
-    <row r="790" ht="14.25" customHeight="1"/>
-    <row r="791" ht="14.25" customHeight="1"/>
-    <row r="792" ht="14.25" customHeight="1"/>
-    <row r="793" ht="14.25" customHeight="1"/>
-    <row r="794" ht="14.25" customHeight="1"/>
-    <row r="795" ht="14.25" customHeight="1"/>
-    <row r="796" ht="14.25" customHeight="1"/>
-    <row r="797" ht="14.25" customHeight="1"/>
-    <row r="798" ht="14.25" customHeight="1"/>
-    <row r="799" ht="14.25" customHeight="1"/>
-    <row r="800" ht="14.25" customHeight="1"/>
-    <row r="801" ht="14.25" customHeight="1"/>
-    <row r="802" ht="14.25" customHeight="1"/>
-    <row r="803" ht="14.25" customHeight="1"/>
-    <row r="804" ht="14.25" customHeight="1"/>
-    <row r="805" ht="14.25" customHeight="1"/>
-    <row r="806" ht="14.25" customHeight="1"/>
-    <row r="807" ht="14.25" customHeight="1"/>
-    <row r="808" ht="14.25" customHeight="1"/>
-    <row r="809" ht="14.25" customHeight="1"/>
-    <row r="810" ht="14.25" customHeight="1"/>
-    <row r="811" ht="14.25" customHeight="1"/>
-    <row r="812" ht="14.25" customHeight="1"/>
-    <row r="813" ht="14.25" customHeight="1"/>
-    <row r="814" ht="14.25" customHeight="1"/>
-    <row r="815" ht="14.25" customHeight="1"/>
-    <row r="816" ht="14.25" customHeight="1"/>
-    <row r="817" ht="14.25" customHeight="1"/>
-    <row r="818" ht="14.25" customHeight="1"/>
-    <row r="819" ht="14.25" customHeight="1"/>
-    <row r="820" ht="14.25" customHeight="1"/>
-    <row r="821" ht="14.25" customHeight="1"/>
-    <row r="822" ht="14.25" customHeight="1"/>
-    <row r="823" ht="14.25" customHeight="1"/>
-    <row r="824" ht="14.25" customHeight="1"/>
-    <row r="825" ht="14.25" customHeight="1"/>
-    <row r="826" ht="14.25" customHeight="1"/>
-    <row r="827" ht="14.25" customHeight="1"/>
-    <row r="828" ht="14.25" customHeight="1"/>
-    <row r="829" ht="14.25" customHeight="1"/>
-    <row r="830" ht="14.25" customHeight="1"/>
-    <row r="831" ht="14.25" customHeight="1"/>
-    <row r="832" ht="14.25" customHeight="1"/>
-    <row r="833" ht="14.25" customHeight="1"/>
-    <row r="834" ht="14.25" customHeight="1"/>
-    <row r="835" ht="14.25" customHeight="1"/>
-    <row r="836" ht="14.25" customHeight="1"/>
-    <row r="837" ht="14.25" customHeight="1"/>
-    <row r="838" ht="14.25" customHeight="1"/>
-    <row r="839" ht="14.25" customHeight="1"/>
-    <row r="840" ht="14.25" customHeight="1"/>
-    <row r="841" ht="14.25" customHeight="1"/>
-    <row r="842" ht="14.25" customHeight="1"/>
-    <row r="843" ht="14.25" customHeight="1"/>
-    <row r="844" ht="14.25" customHeight="1"/>
-    <row r="845" ht="14.25" customHeight="1"/>
-    <row r="846" ht="14.25" customHeight="1"/>
-    <row r="847" ht="14.25" customHeight="1"/>
-    <row r="848" ht="14.25" customHeight="1"/>
-    <row r="849" ht="14.25" customHeight="1"/>
-    <row r="850" ht="14.25" customHeight="1"/>
-    <row r="851" ht="14.25" customHeight="1"/>
-    <row r="852" ht="14.25" customHeight="1"/>
-    <row r="853" ht="14.25" customHeight="1"/>
-    <row r="854" ht="14.25" customHeight="1"/>
-    <row r="855" ht="14.25" customHeight="1"/>
-    <row r="856" ht="14.25" customHeight="1"/>
-    <row r="857" ht="14.25" customHeight="1"/>
-    <row r="858" ht="14.25" customHeight="1"/>
-    <row r="859" ht="14.25" customHeight="1"/>
-    <row r="860" ht="14.25" customHeight="1"/>
-    <row r="861" ht="14.25" customHeight="1"/>
-    <row r="862" ht="14.25" customHeight="1"/>
-    <row r="863" ht="14.25" customHeight="1"/>
-    <row r="864" ht="14.25" customHeight="1"/>
-    <row r="865" ht="14.25" customHeight="1"/>
-    <row r="866" ht="14.25" customHeight="1"/>
-    <row r="867" ht="14.25" customHeight="1"/>
-    <row r="868" ht="14.25" customHeight="1"/>
-    <row r="869" ht="14.25" customHeight="1"/>
-    <row r="870" ht="14.25" customHeight="1"/>
-    <row r="871" ht="14.25" customHeight="1"/>
-    <row r="872" ht="14.25" customHeight="1"/>
-    <row r="873" ht="14.25" customHeight="1"/>
-    <row r="874" ht="14.25" customHeight="1"/>
-    <row r="875" ht="14.25" customHeight="1"/>
-    <row r="876" ht="14.25" customHeight="1"/>
-    <row r="877" ht="14.25" customHeight="1"/>
-    <row r="878" ht="14.25" customHeight="1"/>
-    <row r="879" ht="14.25" customHeight="1"/>
-    <row r="880" ht="14.25" customHeight="1"/>
-    <row r="881" ht="14.25" customHeight="1"/>
-    <row r="882" ht="14.25" customHeight="1"/>
-    <row r="883" ht="14.25" customHeight="1"/>
-    <row r="884" ht="14.25" customHeight="1"/>
-    <row r="885" ht="14.25" customHeight="1"/>
-    <row r="886" ht="14.25" customHeight="1"/>
-    <row r="887" ht="14.25" customHeight="1"/>
-    <row r="888" ht="14.25" customHeight="1"/>
-    <row r="889" ht="14.25" customHeight="1"/>
-    <row r="890" ht="14.25" customHeight="1"/>
-    <row r="891" ht="14.25" customHeight="1"/>
-    <row r="892" ht="14.25" customHeight="1"/>
-    <row r="893" ht="14.25" customHeight="1"/>
-    <row r="894" ht="14.25" customHeight="1"/>
-    <row r="895" ht="14.25" customHeight="1"/>
-    <row r="896" ht="14.25" customHeight="1"/>
-    <row r="897" ht="14.25" customHeight="1"/>
-    <row r="898" ht="14.25" customHeight="1"/>
-    <row r="899" ht="14.25" customHeight="1"/>
-    <row r="900" ht="14.25" customHeight="1"/>
-    <row r="901" ht="14.25" customHeight="1"/>
-    <row r="902" ht="14.25" customHeight="1"/>
-    <row r="903" ht="14.25" customHeight="1"/>
-    <row r="904" ht="14.25" customHeight="1"/>
-    <row r="905" ht="14.25" customHeight="1"/>
-    <row r="906" ht="14.25" customHeight="1"/>
-    <row r="907" ht="14.25" customHeight="1"/>
-    <row r="908" ht="14.25" customHeight="1"/>
-    <row r="909" ht="14.25" customHeight="1"/>
-    <row r="910" ht="14.25" customHeight="1"/>
-    <row r="911" ht="14.25" customHeight="1"/>
-    <row r="912" ht="14.25" customHeight="1"/>
-    <row r="913" ht="14.25" customHeight="1"/>
-    <row r="914" ht="14.25" customHeight="1"/>
-    <row r="915" ht="14.25" customHeight="1"/>
-    <row r="916" ht="14.25" customHeight="1"/>
-    <row r="917" ht="14.25" customHeight="1"/>
-    <row r="918" ht="14.25" customHeight="1"/>
-    <row r="919" ht="14.25" customHeight="1"/>
-    <row r="920" ht="14.25" customHeight="1"/>
-    <row r="921" ht="14.25" customHeight="1"/>
-    <row r="922" ht="14.25" customHeight="1"/>
-    <row r="923" ht="14.25" customHeight="1"/>
-    <row r="924" ht="14.25" customHeight="1"/>
-    <row r="925" ht="14.25" customHeight="1"/>
-    <row r="926" ht="14.25" customHeight="1"/>
-    <row r="927" ht="14.25" customHeight="1"/>
-    <row r="928" ht="14.25" customHeight="1"/>
-    <row r="929" ht="14.25" customHeight="1"/>
-    <row r="930" ht="14.25" customHeight="1"/>
-    <row r="931" ht="14.25" customHeight="1"/>
-    <row r="932" ht="14.25" customHeight="1"/>
-    <row r="933" ht="14.25" customHeight="1"/>
-    <row r="934" ht="14.25" customHeight="1"/>
-    <row r="935" ht="14.25" customHeight="1"/>
-    <row r="936" ht="14.25" customHeight="1"/>
-    <row r="937" ht="14.25" customHeight="1"/>
-    <row r="938" ht="14.25" customHeight="1"/>
-    <row r="939" ht="14.25" customHeight="1"/>
-    <row r="940" ht="14.25" customHeight="1"/>
-    <row r="941" ht="14.25" customHeight="1"/>
-    <row r="942" ht="14.25" customHeight="1"/>
-    <row r="943" ht="14.25" customHeight="1"/>
-    <row r="944" ht="14.25" customHeight="1"/>
-    <row r="945" ht="14.25" customHeight="1"/>
-    <row r="946" ht="14.25" customHeight="1"/>
-    <row r="947" ht="14.25" customHeight="1"/>
-    <row r="948" ht="14.25" customHeight="1"/>
-    <row r="949" ht="14.25" customHeight="1"/>
-    <row r="950" ht="14.25" customHeight="1"/>
-    <row r="951" ht="14.25" customHeight="1"/>
-    <row r="952" ht="14.25" customHeight="1"/>
-    <row r="953" ht="14.25" customHeight="1"/>
-    <row r="954" ht="14.25" customHeight="1"/>
-    <row r="955" ht="14.25" customHeight="1"/>
-    <row r="956" ht="14.25" customHeight="1"/>
-    <row r="957" ht="14.25" customHeight="1"/>
-    <row r="958" ht="14.25" customHeight="1"/>
-    <row r="959" ht="14.25" customHeight="1"/>
-    <row r="960" ht="14.25" customHeight="1"/>
-    <row r="961" ht="14.25" customHeight="1"/>
-    <row r="962" ht="14.25" customHeight="1"/>
-    <row r="963" ht="14.25" customHeight="1"/>
-    <row r="964" ht="14.25" customHeight="1"/>
-    <row r="965" ht="14.25" customHeight="1"/>
-    <row r="966" ht="14.25" customHeight="1"/>
-    <row r="967" ht="14.25" customHeight="1"/>
-    <row r="968" ht="14.25" customHeight="1"/>
-    <row r="969" ht="14.25" customHeight="1"/>
-    <row r="970" ht="14.25" customHeight="1"/>
-    <row r="971" ht="14.25" customHeight="1"/>
-    <row r="972" ht="14.25" customHeight="1"/>
-    <row r="973" ht="14.25" customHeight="1"/>
-    <row r="974" ht="14.25" customHeight="1"/>
-    <row r="975" ht="14.25" customHeight="1"/>
-    <row r="976" ht="14.25" customHeight="1"/>
-    <row r="977" ht="14.25" customHeight="1"/>
-    <row r="978" ht="14.25" customHeight="1"/>
-    <row r="979" ht="14.25" customHeight="1"/>
-    <row r="980" ht="14.25" customHeight="1"/>
-    <row r="981" ht="14.25" customHeight="1"/>
-    <row r="982" ht="14.25" customHeight="1"/>
-    <row r="983" ht="14.25" customHeight="1"/>
-    <row r="984" ht="14.25" customHeight="1"/>
-    <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
-    <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
-    <row r="989" ht="14.25" customHeight="1"/>
-    <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-  </sheetData>
-  <phoneticPr fontId="2"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z987"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-    </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>26</v>
+      <c r="C2" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1648,7 +1643,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1670,7 +1665,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -1681,7 +1676,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1692,7 +1687,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2682,16 +2677,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.86328125" customWidth="1"/>
+    <col min="2" max="2" width="30.1328125" customWidth="1"/>
+    <col min="3" max="3" width="60.265625" customWidth="1"/>
+    <col min="4" max="26" width="65.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2702,7 +2697,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>